<commit_message>
viernes en la tarde
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="BD" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Hoja3" sheetId="2" r:id="rId2"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
+  <sheets>
+    <sheet name="BD" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Hoja3" sheetId="2" state="visible" r:id="rId2"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44,7 +44,7 @@
     <t>O/C:</t>
   </si>
   <si>
-    <t>ODC 03</t>
+    <t>ODC 02</t>
   </si>
   <si>
     <t>Solicitado por</t>
@@ -59,13 +59,13 @@
     <t>Descripción OC</t>
   </si>
   <si>
-    <t>Extensión 2017</t>
+    <t>Laboratorio</t>
   </si>
   <si>
     <t>CentroCosto OC</t>
   </si>
   <si>
-    <t>51-11-3309: Corporate charges_</t>
+    <t>51-11-3315: Office Vallenar_</t>
   </si>
   <si>
     <t>Dueño Ccostos</t>
@@ -655,251 +655,251 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="111">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="1"/>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="2" xfId="2">
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="1"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="3" fontId="8" numFmtId="0" xfId="5">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="3" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="7" fillId="3" fontId="8" numFmtId="0" xfId="5">
+    <xf applyAlignment="1" applyProtection="1" borderId="7" fillId="3" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="14" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="14" fillId="0" fontId="6" numFmtId="0" xfId="5">
+    <xf applyAlignment="1" applyProtection="1" borderId="14" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="17" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="6" numFmtId="165" xfId="1">
+    <xf applyAlignment="1" borderId="14" fillId="0" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="14" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="14" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="6" numFmtId="164" xfId="3">
+    <xf applyAlignment="1" borderId="14" fillId="0" fontId="6" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="166" xfId="1"/>
-    <xf borderId="7" fillId="0" fontId="8" numFmtId="165" xfId="1"/>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="167" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="167" xfId="1"/>
-    <xf borderId="21" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyProtection="1" borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="5">
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="7" fillId="0" fontId="8" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="21" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyProtection="1" borderId="8" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf borderId="22" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyProtection="1" borderId="13" fillId="4" fontId="8" numFmtId="0" xfId="5">
+    <xf borderId="22" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyProtection="1" borderId="13" fillId="4" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="12" fillId="4" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="7" fillId="4" fontId="4" numFmtId="0" xfId="1"/>
-    <xf applyProtection="1" borderId="18" fillId="0" fontId="6" numFmtId="0" xfId="5">
+    <xf borderId="7" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="12" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="7" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyProtection="1" borderId="18" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="167" xfId="3"/>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="168" xfId="4"/>
-    <xf applyProtection="1" borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="5">
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf applyProtection="1" borderId="8" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="14" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="167" xfId="3"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="168" xfId="4"/>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="5">
+    <xf borderId="17" fillId="0" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="18" fillId="0" fontId="8" numFmtId="0" xfId="5">
+    <xf applyProtection="1" borderId="18" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="167" xfId="3"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="167" xfId="1"/>
-    <xf borderId="17" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="168" xfId="4"/>
-    <xf applyProtection="1" borderId="19" fillId="0" fontId="8" numFmtId="0" xfId="5">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="17" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf applyProtection="1" borderId="19" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="167" xfId="1"/>
-    <xf borderId="20" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="1">
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="20" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="5">
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="1"/>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="12" fillId="3" fontId="8" numFmtId="0" xfId="5">
+    <xf borderId="6" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" applyProtection="1" borderId="12" fillId="3" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="6"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="169" pivotButton="0" quotePrefix="0" xfId="6"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="21" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="21" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="22" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="22" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="24" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="24" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="25" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="25" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="26" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="26" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="6" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="18" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="17" fillId="0" fontId="6" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="17" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="6" numFmtId="164" xfId="3">
+    <xf applyAlignment="1" borderId="18" fillId="0" fontId="6" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="17" fillId="0" fontId="6" numFmtId="164" xfId="3">
+    <xf applyAlignment="1" borderId="17" fillId="0" fontId="6" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="19" fillId="0" fontId="6" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="19" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="20" fillId="0" fontId="6" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="20" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="19" fillId="0" fontId="6" numFmtId="165" xfId="1">
+    <xf applyAlignment="1" borderId="19" fillId="0" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="20" fillId="0" fontId="6" numFmtId="165" xfId="1">
+    <xf applyAlignment="1" borderId="20" fillId="0" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="8" numFmtId="164" xfId="3">
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="8" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="12" fillId="0" fontId="8" numFmtId="164" xfId="3">
+    <xf applyAlignment="1" borderId="12" fillId="0" fontId="8" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="8" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="15" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="16" fillId="0" fontId="8" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="16" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="6" numFmtId="165" xfId="1">
+    <xf applyAlignment="1" borderId="15" fillId="0" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="16" fillId="0" fontId="6" numFmtId="165" xfId="1">
+    <xf applyAlignment="1" borderId="16" fillId="0" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="13" fillId="3" fontId="8" numFmtId="0" xfId="5">
+    <xf applyAlignment="1" applyProtection="1" borderId="13" fillId="3" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="12" fillId="3" fontId="8" numFmtId="0" xfId="5">
+    <xf applyAlignment="1" applyProtection="1" borderId="12" fillId="3" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="3" numFmtId="14" xfId="1">
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="6"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="170" pivotButton="0" quotePrefix="0" xfId="6"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="170" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal 2" xfId="0"/>
@@ -910,7 +910,6 @@
     <cellStyle name="Across 46 3" xfId="5"/>
     <cellStyle name="Center 23" xfId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -1188,7 +1187,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="18.83203125"/>
   </cols>
@@ -1249,9 +1248,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="110" t="n">
-        <v>42815</v>
-      </c>
+      <c r="B12" s="110" t="n"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
@@ -1308,7 +1305,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="n">
-        <v>6000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1316,7 +1313,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="n">
-        <v>1000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1332,7 +1329,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="109" t="n">
-        <v>43089</v>
+        <v>43074</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1340,7 +1337,7 @@
         <v>27</v>
       </c>
       <c r="B24" s="109" t="n">
-        <v>43089</v>
+        <v>43070</v>
       </c>
     </row>
   </sheetData>
@@ -1521,12 +1518,9 @@
       <c r="E9" s="105" t="e">
         <v>#REF!</v>
       </c>
-      <c r="F9" s="105" t="n"/>
-      <c r="G9" s="105" t="n"/>
       <c r="H9" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="106" t="n"/>
       <c r="J9" s="11" t="e">
         <v>#REF!</v>
       </c>
@@ -1609,17 +1603,6 @@
       <c r="C14" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="107" t="n"/>
-      <c r="E14" s="107" t="n"/>
-      <c r="F14" s="107" t="n"/>
-      <c r="G14" s="107" t="n"/>
-      <c r="H14" s="107" t="n"/>
-      <c r="I14" s="107" t="n"/>
-      <c r="J14" s="107" t="n"/>
-      <c r="K14" s="107" t="n"/>
-      <c r="L14" s="107" t="n"/>
-      <c r="M14" s="107" t="n"/>
-      <c r="N14" s="108" t="n"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="n"/>
@@ -1627,17 +1610,6 @@
       <c r="C15" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="107" t="n"/>
-      <c r="E15" s="107" t="n"/>
-      <c r="F15" s="107" t="n"/>
-      <c r="G15" s="107" t="n"/>
-      <c r="H15" s="107" t="n"/>
-      <c r="I15" s="107" t="n"/>
-      <c r="J15" s="107" t="n"/>
-      <c r="K15" s="107" t="n"/>
-      <c r="L15" s="107" t="n"/>
-      <c r="M15" s="107" t="n"/>
-      <c r="N15" s="108" t="n"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="n"/>
@@ -1645,17 +1617,6 @@
       <c r="C16" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="107" t="n"/>
-      <c r="E16" s="107" t="n"/>
-      <c r="F16" s="107" t="n"/>
-      <c r="G16" s="107" t="n"/>
-      <c r="H16" s="107" t="n"/>
-      <c r="I16" s="107" t="n"/>
-      <c r="J16" s="107" t="n"/>
-      <c r="K16" s="107" t="n"/>
-      <c r="L16" s="107" t="n"/>
-      <c r="M16" s="107" t="n"/>
-      <c r="N16" s="108" t="n"/>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="2" t="n"/>
@@ -1736,7 +1697,6 @@
       <c r="L20" s="103" t="e">
         <v>#REF!</v>
       </c>
-      <c r="M20" s="104" t="n"/>
       <c r="N20" s="9" t="n"/>
     </row>
     <row r="21" spans="1:14">
@@ -1746,15 +1706,10 @@
       <c r="D21" s="98" t="e">
         <v>#REF!</v>
       </c>
-      <c r="E21" s="99" t="n"/>
-      <c r="F21" s="99" t="n"/>
-      <c r="G21" s="99" t="n"/>
-      <c r="H21" s="100" t="n"/>
       <c r="I21" s="24" t="n"/>
       <c r="J21" s="25" t="n"/>
       <c r="K21" s="26" t="n"/>
       <c r="L21" s="101" t="n"/>
-      <c r="M21" s="102" t="n"/>
       <c r="N21" s="9" t="n"/>
     </row>
     <row r="22" spans="1:14">
@@ -1766,10 +1721,6 @@
       <c r="D22" s="85" t="e">
         <v>#REF!</v>
       </c>
-      <c r="E22" s="86" t="n"/>
-      <c r="F22" s="86" t="n"/>
-      <c r="G22" s="86" t="n"/>
-      <c r="H22" s="87" t="n"/>
       <c r="I22" s="28" t="e">
         <v>#REF!</v>
       </c>
@@ -1782,7 +1733,6 @@
       <c r="L22" s="88" t="e">
         <v>#REF!</v>
       </c>
-      <c r="M22" s="89" t="n"/>
       <c r="N22" s="9" t="n"/>
     </row>
     <row r="23" spans="1:14">
@@ -1790,15 +1740,10 @@
       <c r="B23" s="6" t="n"/>
       <c r="C23" s="27" t="n"/>
       <c r="D23" s="85" t="n"/>
-      <c r="E23" s="86" t="n"/>
-      <c r="F23" s="86" t="n"/>
-      <c r="G23" s="86" t="n"/>
-      <c r="H23" s="87" t="n"/>
       <c r="I23" s="28" t="n"/>
       <c r="J23" s="25" t="n"/>
       <c r="K23" s="29" t="n"/>
       <c r="L23" s="88" t="n"/>
-      <c r="M23" s="89" t="n"/>
       <c r="N23" s="9" t="n"/>
     </row>
     <row r="24" spans="1:14">
@@ -1806,15 +1751,10 @@
       <c r="B24" s="6" t="n"/>
       <c r="C24" s="27" t="n"/>
       <c r="D24" s="85" t="n"/>
-      <c r="E24" s="86" t="n"/>
-      <c r="F24" s="86" t="n"/>
-      <c r="G24" s="86" t="n"/>
-      <c r="H24" s="87" t="n"/>
       <c r="I24" s="28" t="n"/>
       <c r="J24" s="25" t="n"/>
       <c r="K24" s="29" t="n"/>
       <c r="L24" s="88" t="n"/>
-      <c r="M24" s="89" t="n"/>
       <c r="N24" s="9" t="n"/>
     </row>
     <row r="25" spans="1:14">
@@ -1822,15 +1762,10 @@
       <c r="B25" s="6" t="n"/>
       <c r="C25" s="27" t="n"/>
       <c r="D25" s="85" t="n"/>
-      <c r="E25" s="86" t="n"/>
-      <c r="F25" s="86" t="n"/>
-      <c r="G25" s="86" t="n"/>
-      <c r="H25" s="87" t="n"/>
       <c r="I25" s="28" t="n"/>
       <c r="J25" s="25" t="n"/>
       <c r="K25" s="29" t="n"/>
       <c r="L25" s="88" t="n"/>
-      <c r="M25" s="89" t="n"/>
       <c r="N25" s="9" t="n"/>
     </row>
     <row r="26" spans="1:14">
@@ -1838,15 +1773,10 @@
       <c r="B26" s="6" t="n"/>
       <c r="C26" s="27" t="n"/>
       <c r="D26" s="85" t="n"/>
-      <c r="E26" s="86" t="n"/>
-      <c r="F26" s="86" t="n"/>
-      <c r="G26" s="86" t="n"/>
-      <c r="H26" s="87" t="n"/>
       <c r="I26" s="28" t="n"/>
       <c r="J26" s="25" t="n"/>
       <c r="K26" s="29" t="n"/>
       <c r="L26" s="88" t="n"/>
-      <c r="M26" s="89" t="n"/>
       <c r="N26" s="9" t="n"/>
     </row>
     <row r="27" spans="1:14">
@@ -1854,15 +1784,10 @@
       <c r="B27" s="6" t="n"/>
       <c r="C27" s="23" t="n"/>
       <c r="D27" s="90" t="n"/>
-      <c r="E27" s="91" t="n"/>
-      <c r="F27" s="91" t="n"/>
-      <c r="G27" s="91" t="n"/>
-      <c r="H27" s="92" t="n"/>
       <c r="I27" s="28" t="n"/>
       <c r="J27" s="25" t="n"/>
       <c r="K27" s="26" t="n"/>
       <c r="L27" s="93" t="n"/>
-      <c r="M27" s="94" t="n"/>
       <c r="N27" s="9" t="n"/>
     </row>
     <row r="28" spans="1:14">
@@ -1882,7 +1807,6 @@
       <c r="L28" s="95" t="e">
         <v>#REF!</v>
       </c>
-      <c r="M28" s="96" t="n"/>
       <c r="N28" s="9" t="n"/>
     </row>
     <row r="29" spans="1:14">
@@ -2369,18 +2293,12 @@
       <c r="C54" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D54" s="1" t="n"/>
-      <c r="E54" s="1" t="n"/>
       <c r="F54" s="2" t="n"/>
       <c r="G54" s="2" t="n"/>
       <c r="H54" s="2" t="n"/>
       <c r="I54" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="J54" s="97" t="n"/>
-      <c r="K54" s="97" t="n"/>
-      <c r="L54" s="97" t="n"/>
-      <c r="M54" s="97" t="n"/>
       <c r="N54" s="9" t="n"/>
     </row>
     <row r="55" spans="1:14">
@@ -2389,18 +2307,12 @@
       <c r="C55" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="D55" s="84" t="n"/>
-      <c r="E55" s="84" t="n"/>
       <c r="F55" s="2" t="n"/>
       <c r="G55" s="2" t="n"/>
       <c r="H55" s="2" t="n"/>
       <c r="I55" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="J55" s="84" t="n"/>
-      <c r="K55" s="84" t="n"/>
-      <c r="L55" s="84" t="n"/>
-      <c r="M55" s="84" t="n"/>
       <c r="N55" s="9" t="n"/>
     </row>
     <row r="56" spans="1:14">
@@ -2439,16 +2351,10 @@
       <c r="A58" s="2" t="n"/>
       <c r="B58" s="6" t="n"/>
       <c r="C58" s="1" t="n"/>
-      <c r="D58" s="1" t="n"/>
-      <c r="E58" s="1" t="n"/>
       <c r="F58" s="11" t="n"/>
       <c r="G58" s="2" t="n"/>
       <c r="H58" s="2" t="n"/>
       <c r="I58" s="72" t="n"/>
-      <c r="J58" s="72" t="n"/>
-      <c r="K58" s="72" t="n"/>
-      <c r="L58" s="72" t="n"/>
-      <c r="M58" s="72" t="n"/>
       <c r="N58" s="9" t="n"/>
     </row>
     <row r="59" spans="1:14">
@@ -2457,16 +2363,7 @@
       <c r="C59" s="73" t="e">
         <v>#REF!</v>
       </c>
-      <c r="D59" s="73" t="n"/>
-      <c r="E59" s="73" t="n"/>
-      <c r="F59" s="73" t="n"/>
-      <c r="G59" s="73" t="n"/>
-      <c r="H59" s="73" t="n"/>
       <c r="I59" s="74" t="n"/>
-      <c r="J59" s="74" t="n"/>
-      <c r="K59" s="74" t="n"/>
-      <c r="L59" s="74" t="n"/>
-      <c r="M59" s="74" t="n"/>
       <c r="N59" s="9" t="n"/>
     </row>
     <row r="60" spans="1:14">
@@ -2490,66 +2387,15 @@
       <c r="B61" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="76" t="n"/>
-      <c r="D61" s="76" t="n"/>
-      <c r="E61" s="76" t="n"/>
-      <c r="F61" s="76" t="n"/>
-      <c r="G61" s="76" t="n"/>
-      <c r="H61" s="76" t="n"/>
-      <c r="I61" s="76" t="n"/>
-      <c r="J61" s="76" t="n"/>
-      <c r="K61" s="76" t="n"/>
-      <c r="L61" s="76" t="n"/>
-      <c r="M61" s="76" t="n"/>
-      <c r="N61" s="77" t="n"/>
     </row>
     <row r="62" spans="1:14">
       <c r="A62" s="2" t="n"/>
-      <c r="B62" s="78" t="n"/>
-      <c r="C62" s="79" t="n"/>
-      <c r="D62" s="79" t="n"/>
-      <c r="E62" s="79" t="n"/>
-      <c r="F62" s="79" t="n"/>
-      <c r="G62" s="79" t="n"/>
-      <c r="H62" s="79" t="n"/>
-      <c r="I62" s="79" t="n"/>
-      <c r="J62" s="79" t="n"/>
-      <c r="K62" s="79" t="n"/>
-      <c r="L62" s="79" t="n"/>
-      <c r="M62" s="79" t="n"/>
-      <c r="N62" s="80" t="n"/>
     </row>
     <row r="63" spans="1:14">
       <c r="A63" s="2" t="n"/>
-      <c r="B63" s="78" t="n"/>
-      <c r="C63" s="79" t="n"/>
-      <c r="D63" s="79" t="n"/>
-      <c r="E63" s="79" t="n"/>
-      <c r="F63" s="79" t="n"/>
-      <c r="G63" s="79" t="n"/>
-      <c r="H63" s="79" t="n"/>
-      <c r="I63" s="79" t="n"/>
-      <c r="J63" s="79" t="n"/>
-      <c r="K63" s="79" t="n"/>
-      <c r="L63" s="79" t="n"/>
-      <c r="M63" s="79" t="n"/>
-      <c r="N63" s="80" t="n"/>
     </row>
     <row customHeight="1" ht="17" r="64" spans="1:14">
       <c r="A64" s="2" t="n"/>
-      <c r="B64" s="81" t="n"/>
-      <c r="C64" s="82" t="n"/>
-      <c r="D64" s="82" t="n"/>
-      <c r="E64" s="82" t="n"/>
-      <c r="F64" s="82" t="n"/>
-      <c r="G64" s="82" t="n"/>
-      <c r="H64" s="82" t="n"/>
-      <c r="I64" s="82" t="n"/>
-      <c r="J64" s="82" t="n"/>
-      <c r="K64" s="82" t="n"/>
-      <c r="L64" s="82" t="n"/>
-      <c r="M64" s="82" t="n"/>
-      <c r="N64" s="83" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="30">

</xml_diff>

<commit_message>
martes en la tarde
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelleyton/MiDjango/Proy_Python3/tutorial_P3_4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.leyton\MiDjango_\tutorial_P3_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26400" yWindow="7360" windowWidth="28560" windowHeight="17380" activeTab="2"/>
+    <workbookView xWindow="26400" yWindow="7365" windowWidth="28560" windowHeight="17385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BD" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">Commitment!$B$2:$Q$68</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Orden Cambio'!$B$2:$N$69</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="204">
   <si>
     <t>N° de Contrato</t>
   </si>
@@ -513,9 +513,6 @@
     <t xml:space="preserve">Notas: </t>
   </si>
   <si>
-    <t>Valor Neto (CLP) :</t>
-  </si>
-  <si>
     <t>(1) Esta orden de cambio representa el ajuste final para todos y cada uno de los montos adeudados o que se adeudaren al Contratista por los cambios identificados en e ste documento, incluyendo cualquier efecto que ellos pudieran tener en la planificación, programación, obligaciones o compromisos del contratista.</t>
   </si>
   <si>
@@ -528,18 +525,9 @@
     <t>(2) Todas las demas condiciones del contrato, permanecen inalterables.</t>
   </si>
   <si>
-    <t>TOTAL ACTUALIZACIÓN (CLP) :</t>
-  </si>
-  <si>
-    <t>TOTAL ORDEN DE SERVICIO EN CLP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Términos  y Notas de la O.S.: </t>
   </si>
   <si>
-    <t>MONTO INICIAL OS-2016-048 :</t>
-  </si>
-  <si>
     <t>Fecha de Inicio del Servicio:</t>
   </si>
   <si>
@@ -658,9 +646,6 @@
   </si>
   <si>
     <t xml:space="preserve">Falta solicitante, </t>
-  </si>
-  <si>
-    <t>TOTAL ACUM NETO OS-2016-048:</t>
   </si>
   <si>
     <t>Cargo Dueño Ccostos</t>
@@ -669,24 +654,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="14">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0;\-&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot; &quot;_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="#,##0.0"/>
-    <numFmt numFmtId="174" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;&quot;?_);_(@_)"/>
-    <numFmt numFmtId="175" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0;\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot; &quot;_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="#,##0.0"/>
+    <numFmt numFmtId="173" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;&quot;?_);_(@_)"/>
+    <numFmt numFmtId="174" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -980,6 +965,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -1078,7 +1069,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="64">
+  <borders count="65">
     <border>
       <left/>
       <right/>
@@ -1839,6 +1830,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1850,15 +1852,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="524">
+  <cellXfs count="527">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1904,13 +1906,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1926,26 +1928,26 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1977,11 +1979,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1996,37 +1998,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="17" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="17" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="16" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="16" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2038,7 +2040,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2184,7 +2186,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="31" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="29" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2259,7 +2261,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="16" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2274,7 +2276,7 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="16" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="16" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2352,7 +2354,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="16" fillId="0" borderId="29" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="29" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2381,10 +2383,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="173" fontId="25" fillId="0" borderId="40" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="25" fillId="0" borderId="40" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="19" fillId="2" borderId="34" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="172" fontId="19" fillId="2" borderId="34" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="16" fillId="9" borderId="34" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="8" borderId="18" xfId="8" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="justify" wrapText="1"/>
@@ -2567,18 +2569,15 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="15" fillId="8" borderId="52" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="15" fillId="8" borderId="52" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="175" fontId="15" fillId="8" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="175" fontId="15" fillId="8" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="15" fillId="8" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="174" fontId="15" fillId="8" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="33" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2704,13 +2703,13 @@
     <xf numFmtId="0" fontId="39" fillId="6" borderId="37" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="13" fillId="6" borderId="44" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="13" fillId="6" borderId="44" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="6" borderId="44" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="13" fillId="6" borderId="44" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="13" fillId="6" borderId="44" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="44" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2725,11 +2724,11 @@
     <xf numFmtId="0" fontId="26" fillId="6" borderId="55" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="13" fillId="6" borderId="56" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="13" fillId="6" borderId="56" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="8" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="15" fillId="8" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="15" fillId="8" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2739,18 +2738,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="42" fillId="15" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="33" fillId="15" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="15" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="33" fillId="15" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="8" applyFont="1" applyBorder="1"/>
@@ -2771,10 +2758,10 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="174" fontId="13" fillId="6" borderId="42" xfId="8" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="13" fillId="6" borderId="42" xfId="8" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="13" fillId="6" borderId="43" xfId="8" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="13" fillId="6" borderId="43" xfId="8" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="37" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2799,16 +2786,13 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="175" fontId="19" fillId="8" borderId="46" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="19" fillId="8" borderId="43" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="19" fillId="8" borderId="43" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="15" fillId="8" borderId="52" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="15" fillId="8" borderId="52" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="175" fontId="15" fillId="8" borderId="53" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="15" fillId="8" borderId="53" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2829,7 +2813,7 @@
     <xf numFmtId="2" fontId="19" fillId="0" borderId="52" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="175" fontId="15" fillId="8" borderId="53" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="174" fontId="15" fillId="8" borderId="53" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="62" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2895,22 +2879,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="13" fillId="6" borderId="59" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="13" fillId="6" borderId="59" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="57" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="13" fillId="0" borderId="57" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="16" fillId="8" borderId="60" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="16" fillId="8" borderId="60" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="16" fillId="8" borderId="51" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="16" fillId="8" borderId="51" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="16" fillId="8" borderId="61" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="16" fillId="8" borderId="61" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="11" borderId="50" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="15" fillId="11" borderId="50" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2982,6 +2966,14 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="174" fontId="19" fillId="8" borderId="47" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2998,13 +2990,13 @@
     <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="175" fontId="16" fillId="8" borderId="46" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="16" fillId="8" borderId="46" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="16" fillId="8" borderId="43" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="16" fillId="8" borderId="43" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="16" fillId="8" borderId="47" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="16" fillId="8" borderId="47" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3013,27 +3005,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3049,7 +3020,7 @@
     <xf numFmtId="14" fontId="26" fillId="15" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="16" fillId="9" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3082,8 +3053,44 @@
     <xf numFmtId="3" fontId="16" fillId="9" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="42" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="42" fillId="15" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="42" fillId="15" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="42" fillId="15" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="15" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -3414,36 +3421,36 @@
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="58" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" style="58" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H4" s="271" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="92"/>
       <c r="H5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3452,28 +3459,28 @@
       </c>
       <c r="B6" s="92"/>
       <c r="H6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I6" t="s">
         <v>134</v>
       </c>
       <c r="J6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="92"/>
       <c r="H7" s="295" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I7" t="s">
         <v>137</v>
       </c>
       <c r="J7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3482,7 +3489,7 @@
       </c>
       <c r="B8" s="92"/>
       <c r="H8" s="295" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I8" t="s">
         <v>139</v>
@@ -3491,19 +3498,19 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="92"/>
       <c r="H9" s="295" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I9" t="s">
         <v>142</v>
       </c>
       <c r="J9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3512,25 +3519,25 @@
       </c>
       <c r="B10" s="92"/>
       <c r="H10" s="295" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I10" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="92"/>
       <c r="H11" s="295" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I11" t="s">
         <v>146</v>
       </c>
       <c r="J11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3539,13 +3546,13 @@
       </c>
       <c r="B12" s="93"/>
       <c r="H12" s="295" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3557,15 +3564,15 @@
       </c>
       <c r="B14" s="92"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="92"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B16" s="92"/>
     </row>
@@ -3604,73 +3611,73 @@
       </c>
       <c r="B21" s="92"/>
       <c r="C21" s="275"/>
-      <c r="I21" s="414" t="s">
-        <v>206</v>
-      </c>
-      <c r="J21" s="414"/>
-      <c r="K21" s="414"/>
+      <c r="I21" s="409" t="s">
+        <v>202</v>
+      </c>
+      <c r="J21" s="409"/>
+      <c r="K21" s="409"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="93"/>
-      <c r="I22" s="414"/>
-      <c r="J22" s="414"/>
-      <c r="K22" s="414"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I22" s="409"/>
+      <c r="J22" s="409"/>
+      <c r="K22" s="409"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="93"/>
-      <c r="I23" s="414"/>
-      <c r="J23" s="414"/>
-      <c r="K23" s="414"/>
+      <c r="I23" s="409"/>
+      <c r="J23" s="409"/>
+      <c r="K23" s="409"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="93"/>
-      <c r="I24" s="414"/>
-      <c r="J24" s="414"/>
-      <c r="K24" s="414"/>
+      <c r="I24" s="409"/>
+      <c r="J24" s="409"/>
+      <c r="K24" s="409"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="93"/>
-      <c r="I25" s="414"/>
-      <c r="J25" s="414"/>
-      <c r="K25" s="414"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I25" s="409"/>
+      <c r="J25" s="409"/>
+      <c r="K25" s="409"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="58" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B26" s="92"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B27" s="92"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="58" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B28" s="92"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="58" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B29" s="92"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -3835,7 +3842,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N69"/>
@@ -3844,16 +3851,16 @@
       <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.6640625" style="91" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="91" customWidth="1"/>
+    <col min="2" max="2" width="3.625" style="91" customWidth="1"/>
+    <col min="8" max="8" width="12.625" style="91" customWidth="1"/>
     <col min="12" max="12" width="13" style="91" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" style="91" customWidth="1"/>
-    <col min="14" max="14" width="2.1640625" style="91" customWidth="1"/>
+    <col min="13" max="13" width="14.375" style="91" customWidth="1"/>
+    <col min="14" max="14" width="2.125" style="91" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="89"/>
       <c r="B1" s="89"/>
       <c r="C1" s="89"/>
@@ -3869,7 +3876,7 @@
       <c r="M1" s="89"/>
       <c r="N1" s="89"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
@@ -3885,7 +3892,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="str">
@@ -3897,14 +3904,14 @@
       <c r="F3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="L3" s="523">
+      <c r="L3" s="481">
         <f>BD!B29</f>
         <v>0</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
       <c r="B4" s="5"/>
       <c r="C4" s="89"/>
@@ -3920,7 +3927,7 @@
       <c r="M4" s="89"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="89"/>
       <c r="B5" s="5"/>
       <c r="C5" s="89" t="s">
@@ -3941,7 +3948,7 @@
       <c r="M5" s="89"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
       <c r="B6" s="5"/>
       <c r="C6" s="89" t="s">
@@ -3962,7 +3969,7 @@
       <c r="M6" s="89"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
       <c r="B7" s="5"/>
       <c r="C7" s="89" t="s">
@@ -3988,7 +3995,7 @@
       <c r="M7" s="89"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
       <c r="B8" s="5"/>
       <c r="C8" s="89" t="s">
@@ -4009,30 +4016,30 @@
       <c r="M8" s="89"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
       <c r="B9" s="5"/>
       <c r="C9" s="89" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="89"/>
-      <c r="E9" s="488">
+      <c r="E9" s="486">
         <f ca="1">TODAY()</f>
         <v>42836</v>
       </c>
-      <c r="F9" s="489"/>
-      <c r="G9" s="489"/>
-      <c r="H9" s="490" t="s">
+      <c r="F9" s="487"/>
+      <c r="G9" s="487"/>
+      <c r="H9" s="488" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="489"/>
+      <c r="I9" s="487"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="15"/>
       <c r="M9" s="89"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
       <c r="B10" s="5"/>
       <c r="C10" s="89"/>
@@ -4048,7 +4055,7 @@
       <c r="M10" s="89"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="89"/>
       <c r="B11" s="16"/>
       <c r="C11" s="10"/>
@@ -4064,7 +4071,7 @@
       <c r="M11" s="10"/>
       <c r="N11" s="17"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="89"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
@@ -4080,7 +4087,7 @@
       <c r="M12" s="89"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="89"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6" t="s">
@@ -4098,48 +4105,48 @@
       <c r="M13" s="89"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="89"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="491" t="str">
+      <c r="C14" s="489" t="str">
         <f>"Esta orden de cambio de contrato, tiene como objetivo ajustar el alcance, valor y plazo del Contrato "&amp;E5&amp;" incorporando el alcance de servicio denominado "&amp;E8&amp;" "&amp;BD!B13</f>
         <v xml:space="preserve">Esta orden de cambio de contrato, tiene como objetivo ajustar el alcance, valor y plazo del Contrato 0 incorporando el alcance de servicio denominado 0 </v>
       </c>
-      <c r="D14" s="491"/>
-      <c r="E14" s="491"/>
-      <c r="F14" s="491"/>
-      <c r="G14" s="491"/>
-      <c r="H14" s="491"/>
-      <c r="I14" s="491"/>
-      <c r="J14" s="491"/>
-      <c r="K14" s="491"/>
-      <c r="L14" s="491"/>
-      <c r="M14" s="491"/>
+      <c r="D14" s="489"/>
+      <c r="E14" s="489"/>
+      <c r="F14" s="489"/>
+      <c r="G14" s="489"/>
+      <c r="H14" s="489"/>
+      <c r="I14" s="489"/>
+      <c r="J14" s="489"/>
+      <c r="K14" s="489"/>
+      <c r="L14" s="489"/>
+      <c r="M14" s="489"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="89"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="491"/>
-      <c r="D15" s="491"/>
-      <c r="E15" s="491"/>
-      <c r="F15" s="491"/>
-      <c r="G15" s="491"/>
-      <c r="H15" s="491"/>
-      <c r="I15" s="491"/>
-      <c r="J15" s="491"/>
-      <c r="K15" s="491"/>
-      <c r="L15" s="491"/>
-      <c r="M15" s="491"/>
+      <c r="C15" s="489"/>
+      <c r="D15" s="489"/>
+      <c r="E15" s="489"/>
+      <c r="F15" s="489"/>
+      <c r="G15" s="489"/>
+      <c r="H15" s="489"/>
+      <c r="I15" s="489"/>
+      <c r="J15" s="489"/>
+      <c r="K15" s="489"/>
+      <c r="L15" s="489"/>
+      <c r="M15" s="489"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="89"/>
       <c r="B16" s="5"/>
       <c r="C16" s="62"/>
       <c r="N16" s="8"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="89"/>
       <c r="B17" s="16"/>
       <c r="C17" s="10"/>
@@ -4155,7 +4162,7 @@
       <c r="M17" s="10"/>
       <c r="N17" s="17"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="89"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6" t="str">
@@ -4174,7 +4181,7 @@
       <c r="M18" s="89"/>
       <c r="N18" s="8"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="89"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -4194,7 +4201,7 @@
       </c>
       <c r="N19" s="8"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="89"/>
       <c r="B20" s="5"/>
       <c r="C20" s="20" t="s">
@@ -4225,7 +4232,7 @@
       </c>
       <c r="N20" s="8"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="89"/>
       <c r="B21" s="5"/>
       <c r="C21" s="22"/>
@@ -4239,7 +4246,7 @@
       <c r="M21" s="73"/>
       <c r="N21" s="8"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="89"/>
       <c r="B22" s="5"/>
       <c r="C22" s="76">
@@ -4276,7 +4283,7 @@
       </c>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="89"/>
       <c r="B23" s="5"/>
       <c r="C23" s="76">
@@ -4313,7 +4320,7 @@
       </c>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="89"/>
       <c r="B24" s="5"/>
       <c r="C24" s="76">
@@ -4350,7 +4357,7 @@
       </c>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="89"/>
       <c r="B25" s="5"/>
       <c r="C25" s="76">
@@ -4387,7 +4394,7 @@
       </c>
       <c r="N25" s="8"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="89"/>
       <c r="B26" s="5"/>
       <c r="C26" s="76">
@@ -4424,7 +4431,7 @@
       </c>
       <c r="N26" s="8"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="89"/>
       <c r="B27" s="5"/>
       <c r="C27" s="76">
@@ -4461,7 +4468,7 @@
       </c>
       <c r="N27" s="8"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="89"/>
       <c r="B28" s="5"/>
       <c r="C28" s="76">
@@ -4498,7 +4505,7 @@
       </c>
       <c r="N28" s="8"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="89"/>
       <c r="B29" s="5"/>
       <c r="C29" s="76">
@@ -4535,7 +4542,7 @@
       </c>
       <c r="N29" s="8"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="89"/>
       <c r="B30" s="5"/>
       <c r="C30" s="76">
@@ -4572,7 +4579,7 @@
       </c>
       <c r="N30" s="8"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="89"/>
       <c r="B31" s="5"/>
       <c r="C31" s="76">
@@ -4609,7 +4616,7 @@
       </c>
       <c r="N31" s="8"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="89"/>
       <c r="B32" s="5"/>
       <c r="C32" s="22"/>
@@ -4625,7 +4632,7 @@
       <c r="M32" s="74"/>
       <c r="N32" s="8"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="89"/>
       <c r="B33" s="5"/>
       <c r="C33" s="25"/>
@@ -4646,7 +4653,7 @@
       </c>
       <c r="N33" s="8"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="89"/>
       <c r="B34" s="5"/>
       <c r="C34" s="26" t="s">
@@ -4664,7 +4671,7 @@
       <c r="M34" s="28"/>
       <c r="N34" s="8"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="89"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
@@ -4680,7 +4687,7 @@
       <c r="M35" s="89"/>
       <c r="N35" s="8"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="89"/>
       <c r="B36" s="5"/>
       <c r="C36" s="89"/>
@@ -4696,7 +4703,7 @@
       <c r="M36" s="41"/>
       <c r="N36" s="8"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="89"/>
       <c r="B37" s="29"/>
       <c r="C37" s="30" t="s">
@@ -4714,7 +4721,7 @@
       <c r="M37" s="26"/>
       <c r="N37" s="31"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="89"/>
       <c r="B38" s="5"/>
       <c r="C38" s="32" t="s">
@@ -4734,7 +4741,7 @@
       <c r="M38" s="34"/>
       <c r="N38" s="8"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="89"/>
       <c r="B39" s="5"/>
       <c r="C39" s="36" t="s">
@@ -4767,7 +4774,7 @@
       </c>
       <c r="N39" s="8"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="89"/>
       <c r="B40" s="5"/>
       <c r="C40" s="36" t="s">
@@ -4793,7 +4800,7 @@
       <c r="M40" s="40"/>
       <c r="N40" s="8"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="89"/>
       <c r="B41" s="5"/>
       <c r="C41" s="36" t="s">
@@ -4819,7 +4826,7 @@
       <c r="M41" s="40"/>
       <c r="N41" s="8"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="89"/>
       <c r="B42" s="5"/>
       <c r="C42" s="36"/>
@@ -4835,7 +4842,7 @@
       <c r="M42" s="40"/>
       <c r="N42" s="8"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="89"/>
       <c r="B43" s="5"/>
       <c r="C43" s="36"/>
@@ -4851,7 +4858,7 @@
       <c r="M43" s="37"/>
       <c r="N43" s="8"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="89"/>
       <c r="B44" s="5"/>
       <c r="C44" s="44" t="s">
@@ -4884,7 +4891,7 @@
       </c>
       <c r="N44" s="8"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="89"/>
       <c r="B45" s="5"/>
       <c r="C45" s="48"/>
@@ -4900,7 +4907,7 @@
       <c r="M45" s="50"/>
       <c r="N45" s="8"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="89"/>
       <c r="B46" s="16"/>
       <c r="C46" s="10"/>
@@ -4916,7 +4923,7 @@
       <c r="M46" s="10"/>
       <c r="N46" s="17"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="89"/>
       <c r="B47" s="5"/>
       <c r="C47" s="52" t="s">
@@ -4934,7 +4941,7 @@
       <c r="M47" s="89"/>
       <c r="N47" s="8"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="89"/>
       <c r="B48" s="5"/>
       <c r="C48" s="52"/>
@@ -4950,7 +4957,7 @@
       <c r="M48" s="89"/>
       <c r="N48" s="8"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="89"/>
       <c r="B49" s="5"/>
       <c r="C49" s="89"/>
@@ -4966,7 +4973,7 @@
       <c r="M49" s="89"/>
       <c r="N49" s="8"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="89"/>
       <c r="B50" s="16"/>
       <c r="C50" s="53"/>
@@ -4982,7 +4989,7 @@
       <c r="M50" s="10"/>
       <c r="N50" s="17"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="89"/>
       <c r="B51" s="5"/>
       <c r="C51" s="6" t="s">
@@ -5000,7 +5007,7 @@
       <c r="M51" s="89"/>
       <c r="N51" s="8"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="89"/>
       <c r="B52" s="5"/>
       <c r="C52" s="54"/>
@@ -5016,7 +5023,7 @@
       <c r="M52" s="89"/>
       <c r="N52" s="8"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="89"/>
       <c r="B53" s="5"/>
       <c r="C53" s="89" t="s">
@@ -5038,7 +5045,7 @@
       <c r="M53" s="89"/>
       <c r="N53" s="8"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="89"/>
       <c r="B54" s="5"/>
       <c r="C54" s="89" t="s">
@@ -5056,7 +5063,7 @@
       <c r="M54" s="89"/>
       <c r="N54" s="8"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="89"/>
       <c r="B55" s="16"/>
       <c r="C55" s="10"/>
@@ -5072,7 +5079,7 @@
       <c r="M55" s="10"/>
       <c r="N55" s="17"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="89"/>
       <c r="B56" s="5"/>
       <c r="C56" s="6" t="s">
@@ -5090,7 +5097,7 @@
       <c r="M56" s="89"/>
       <c r="N56" s="8"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="89"/>
       <c r="B57" s="5"/>
       <c r="C57" s="89"/>
@@ -5106,7 +5113,7 @@
       <c r="M57" s="89"/>
       <c r="N57" s="8"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="89"/>
       <c r="B58" s="5"/>
       <c r="C58" s="89"/>
@@ -5122,7 +5129,7 @@
       <c r="M58" s="89"/>
       <c r="N58" s="8"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="89"/>
       <c r="B59" s="5"/>
       <c r="C59" s="236"/>
@@ -5138,7 +5145,7 @@
       <c r="M59" s="89"/>
       <c r="N59" s="8"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="89"/>
       <c r="B60" s="5"/>
       <c r="C60" s="14" t="str">
@@ -5158,7 +5165,7 @@
       <c r="M60" s="89"/>
       <c r="N60" s="8"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="89"/>
       <c r="B61" s="5"/>
       <c r="C61" s="89"/>
@@ -5174,7 +5181,7 @@
       <c r="M61" s="89"/>
       <c r="N61" s="8"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="89"/>
       <c r="B62" s="5"/>
       <c r="C62" s="89"/>
@@ -5190,7 +5197,7 @@
       <c r="M62" s="89"/>
       <c r="N62" s="8"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="89"/>
       <c r="B63" s="5"/>
       <c r="C63" s="288"/>
@@ -5206,7 +5213,7 @@
       <c r="M63" s="280"/>
       <c r="N63" s="8"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="89"/>
       <c r="B64" s="5"/>
       <c r="D64" s="293">
@@ -5222,7 +5229,7 @@
       <c r="M64" s="280"/>
       <c r="N64" s="8"/>
     </row>
-    <row r="65" spans="1:14" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="89"/>
       <c r="B65" s="5"/>
       <c r="C65" s="89"/>
@@ -5238,7 +5245,7 @@
       <c r="M65" s="90"/>
       <c r="N65" s="8"/>
     </row>
-    <row r="66" spans="1:14" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="89"/>
       <c r="B66" s="285"/>
       <c r="C66" s="286"/>
@@ -5254,25 +5261,25 @@
       <c r="M66" s="276"/>
       <c r="N66" s="277"/>
     </row>
-    <row r="67" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="89"/>
       <c r="B67" s="278"/>
-      <c r="C67" s="487" t="s">
+      <c r="C67" s="485" t="s">
         <v>55</v>
       </c>
-      <c r="D67" s="487"/>
-      <c r="E67" s="487"/>
-      <c r="F67" s="487"/>
-      <c r="G67" s="487"/>
-      <c r="H67" s="487"/>
-      <c r="I67" s="487"/>
-      <c r="J67" s="487"/>
-      <c r="K67" s="487"/>
-      <c r="L67" s="487"/>
-      <c r="M67" s="487"/>
+      <c r="D67" s="485"/>
+      <c r="E67" s="485"/>
+      <c r="F67" s="485"/>
+      <c r="G67" s="485"/>
+      <c r="H67" s="485"/>
+      <c r="I67" s="485"/>
+      <c r="J67" s="485"/>
+      <c r="K67" s="485"/>
+      <c r="L67" s="485"/>
+      <c r="M67" s="485"/>
       <c r="N67" s="281"/>
     </row>
-    <row r="68" spans="1:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="89"/>
       <c r="B68" s="278"/>
       <c r="C68" s="261"/>
@@ -5288,7 +5295,7 @@
       <c r="M68" s="287"/>
       <c r="N68" s="281"/>
     </row>
-    <row r="69" spans="1:14" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="89"/>
       <c r="B69" s="282"/>
       <c r="C69" s="283"/>
@@ -5318,46 +5325,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41:K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="6.875" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="9.625" customWidth="1"/>
+    <col min="5" max="5" width="19.125" customWidth="1"/>
     <col min="6" max="6" width="5.5" customWidth="1"/>
-    <col min="7" max="7" width="5" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" customWidth="1"/>
-    <col min="12" max="12" width="22.1640625" customWidth="1"/>
-    <col min="13" max="13" width="6.1640625" customWidth="1"/>
+    <col min="7" max="7" width="6.25" customWidth="1"/>
+    <col min="8" max="8" width="14.125" customWidth="1"/>
+    <col min="9" max="9" width="12.625" customWidth="1"/>
+    <col min="10" max="10" width="12.125" customWidth="1"/>
+    <col min="11" max="11" width="18.125" customWidth="1"/>
+    <col min="12" max="12" width="22.125" customWidth="1"/>
+    <col min="13" max="13" width="6.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="359"/>
-      <c r="C1" s="360"/>
-      <c r="D1" s="360"/>
-      <c r="E1" s="361"/>
-      <c r="F1" s="361"/>
-      <c r="G1" s="401"/>
-      <c r="H1" s="363"/>
-      <c r="I1" s="363"/>
-      <c r="J1" s="364"/>
-      <c r="K1" s="364"/>
-      <c r="L1" s="365"/>
-    </row>
-    <row r="2" spans="2:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="402" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="358"/>
+      <c r="C1" s="359"/>
+      <c r="D1" s="359"/>
+      <c r="E1" s="360"/>
+      <c r="F1" s="360"/>
+      <c r="G1" s="396"/>
+      <c r="H1" s="362"/>
+      <c r="I1" s="362"/>
+      <c r="J1" s="363"/>
+      <c r="K1" s="363"/>
+      <c r="L1" s="364"/>
+    </row>
+    <row r="2" spans="2:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="397" t="s">
         <v>127</v>
       </c>
       <c r="C2" s="297"/>
@@ -5368,48 +5375,48 @@
       <c r="H2" s="298"/>
       <c r="I2" s="298"/>
       <c r="J2" s="299"/>
-      <c r="K2" s="523">
+      <c r="K2" s="481">
         <f>BD!B29</f>
         <v>0</v>
       </c>
-      <c r="L2" s="368"/>
-    </row>
-    <row r="3" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="403"/>
-      <c r="C3" s="404"/>
-      <c r="D3" s="404"/>
-      <c r="E3" s="376"/>
-      <c r="F3" s="376"/>
-      <c r="G3" s="405"/>
-      <c r="H3" s="378"/>
-      <c r="I3" s="378"/>
-      <c r="J3" s="379"/>
-      <c r="K3" s="379"/>
-      <c r="L3" s="380"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="359"/>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="361"/>
-      <c r="F4" s="361"/>
-      <c r="G4" s="362"/>
-      <c r="H4" s="363"/>
-      <c r="I4" s="363"/>
-      <c r="J4" s="364"/>
-      <c r="K4" s="364"/>
-      <c r="L4" s="365"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="366" t="s">
+      <c r="L2" s="367"/>
+    </row>
+    <row r="3" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="398"/>
+      <c r="C3" s="399"/>
+      <c r="D3" s="399"/>
+      <c r="E3" s="375"/>
+      <c r="F3" s="375"/>
+      <c r="G3" s="400"/>
+      <c r="H3" s="377"/>
+      <c r="I3" s="377"/>
+      <c r="J3" s="378"/>
+      <c r="K3" s="378"/>
+      <c r="L3" s="379"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="358"/>
+      <c r="C4" s="359"/>
+      <c r="D4" s="359"/>
+      <c r="E4" s="360"/>
+      <c r="F4" s="360"/>
+      <c r="G4" s="361"/>
+      <c r="H4" s="362"/>
+      <c r="I4" s="362"/>
+      <c r="J4" s="363"/>
+      <c r="K4" s="363"/>
+      <c r="L4" s="364"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="365" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="463">
+      <c r="C5" s="457">
         <f>BD!B5</f>
         <v>0</v>
       </c>
       <c r="D5" s="303"/>
-      <c r="E5" s="406" t="str">
+      <c r="E5" s="401" t="str">
         <f>"Actualizacion "&amp;MID('Orden Cambio'!E8,5,2)</f>
         <v xml:space="preserve">Actualizacion </v>
       </c>
@@ -5418,29 +5425,29 @@
       <c r="I5" s="314" t="s">
         <v>131</v>
       </c>
-      <c r="J5" s="485">
+      <c r="J5" s="479">
         <f>BD!B14</f>
         <v>0</v>
       </c>
       <c r="K5" s="92"/>
-      <c r="L5" s="484"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="367" t="s">
+      <c r="L5" s="478"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="366" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="492">
+      <c r="C6" s="490">
         <f ca="1">TODAY()</f>
         <v>42836</v>
       </c>
-      <c r="D6" s="492"/>
-      <c r="E6" s="492"/>
-      <c r="F6" s="492"/>
+      <c r="D6" s="490"/>
+      <c r="E6" s="490"/>
+      <c r="F6" s="490"/>
       <c r="G6" s="299"/>
-      <c r="L6" s="368"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="369"/>
+      <c r="L6" s="367"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="368"/>
       <c r="C7" s="300"/>
       <c r="D7" s="300"/>
       <c r="E7" s="300"/>
@@ -5449,10 +5456,10 @@
       <c r="I7" s="306"/>
       <c r="J7" s="309"/>
       <c r="K7" s="309"/>
-      <c r="L7" s="368"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="370" t="s">
+      <c r="L7" s="367"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="369" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="310"/>
@@ -5460,16 +5467,16 @@
       <c r="E8" s="312"/>
       <c r="F8" s="312"/>
       <c r="G8" s="313"/>
-      <c r="I8" s="482" t="s">
-        <v>178</v>
-      </c>
-      <c r="L8" s="368"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="371" t="s">
+      <c r="I8" s="476" t="s">
+        <v>174</v>
+      </c>
+      <c r="L8" s="367"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="370" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="464">
+      <c r="C9" s="458">
         <f>BD!B7</f>
         <v>0</v>
       </c>
@@ -5477,13 +5484,13 @@
       <c r="E9" s="301"/>
       <c r="F9" s="301"/>
       <c r="G9" s="307"/>
-      <c r="I9" s="483" t="s">
+      <c r="I9" s="477" t="s">
         <v>112</v>
       </c>
-      <c r="L9" s="368"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="372" t="s">
+      <c r="L9" s="367"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="371" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="316">
@@ -5494,16 +5501,16 @@
       <c r="E10" s="301"/>
       <c r="F10" s="301"/>
       <c r="G10" s="307"/>
-      <c r="I10" s="338" t="s">
+      <c r="I10" s="337" t="s">
         <v>114</v>
       </c>
-      <c r="L10" s="368"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="372" t="s">
+      <c r="L10" s="367"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="371" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="464">
+      <c r="C11" s="458">
         <f>BD!B26</f>
         <v>0</v>
       </c>
@@ -5511,10 +5518,10 @@
       <c r="E11" s="301"/>
       <c r="F11" s="301"/>
       <c r="G11" s="307"/>
-      <c r="L11" s="368"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="373" t="s">
+      <c r="L11" s="367"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="372" t="s">
         <v>135</v>
       </c>
       <c r="C12" s="317"/>
@@ -5525,15 +5532,15 @@
       <c r="I12" s="296" t="s">
         <v>132</v>
       </c>
-      <c r="J12" s="407" t="str">
+      <c r="J12" s="402" t="str">
         <f>IF(BD!B29="NUEVAUNION SPA","I","J")</f>
         <v>J</v>
       </c>
       <c r="K12" s="315"/>
-      <c r="L12" s="368"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="372" t="s">
+      <c r="L12" s="367"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="371" t="s">
         <v>138</v>
       </c>
       <c r="C13" s="316"/>
@@ -5547,10 +5554,10 @@
       </c>
       <c r="J13" s="316"/>
       <c r="K13" s="316"/>
-      <c r="L13" s="368"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="372" t="s">
+      <c r="L13" s="367"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="371" t="s">
         <v>140</v>
       </c>
       <c r="C14" s="316" t="s">
@@ -5566,10 +5573,10 @@
       </c>
       <c r="J14" s="316"/>
       <c r="K14" s="316"/>
-      <c r="L14" s="368"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="373" t="s">
+      <c r="L14" s="367"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="372" t="s">
         <v>143</v>
       </c>
       <c r="C15" s="317"/>
@@ -5583,10 +5590,10 @@
       </c>
       <c r="J15" s="316"/>
       <c r="K15" s="316"/>
-      <c r="L15" s="368"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="372" t="s">
+      <c r="L15" s="367"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="371" t="s">
         <v>145</v>
       </c>
       <c r="C16" s="318"/>
@@ -5600,10 +5607,10 @@
       </c>
       <c r="J16" s="316"/>
       <c r="K16" s="316"/>
-      <c r="L16" s="368"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="372" t="s">
+      <c r="L16" s="367"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="371" t="s">
         <v>147</v>
       </c>
       <c r="C17" s="319"/>
@@ -5617,10 +5624,10 @@
       </c>
       <c r="J17" s="316"/>
       <c r="K17" s="316"/>
-      <c r="L17" s="368"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="372" t="s">
+      <c r="L17" s="367"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="371" t="s">
         <v>149</v>
       </c>
       <c r="C18" s="316"/>
@@ -5634,10 +5641,10 @@
       </c>
       <c r="J18" s="316"/>
       <c r="K18" s="316"/>
-      <c r="L18" s="368"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="372" t="s">
+      <c r="L18" s="367"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="371" t="s">
         <v>150</v>
       </c>
       <c r="C19" s="320"/>
@@ -5651,10 +5658,10 @@
       </c>
       <c r="J19" s="316"/>
       <c r="K19" s="316"/>
-      <c r="L19" s="368"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="372" t="s">
+      <c r="L19" s="367"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="371" t="s">
         <v>151</v>
       </c>
       <c r="C20" s="320"/>
@@ -5668,59 +5675,59 @@
       </c>
       <c r="J20" s="316"/>
       <c r="K20" s="316"/>
-      <c r="L20" s="368"/>
-    </row>
-    <row r="21" spans="2:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="374"/>
-      <c r="C21" s="375"/>
-      <c r="D21" s="375"/>
-      <c r="E21" s="376"/>
-      <c r="F21" s="376"/>
-      <c r="G21" s="377"/>
-      <c r="H21" s="378"/>
-      <c r="I21" s="378"/>
-      <c r="J21" s="379"/>
-      <c r="K21" s="379"/>
-      <c r="L21" s="380"/>
-    </row>
-    <row r="22" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="387" t="s">
+      <c r="L20" s="367"/>
+    </row>
+    <row r="21" spans="2:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="373"/>
+      <c r="C21" s="374"/>
+      <c r="D21" s="374"/>
+      <c r="E21" s="375"/>
+      <c r="F21" s="375"/>
+      <c r="G21" s="376"/>
+      <c r="H21" s="377"/>
+      <c r="I21" s="377"/>
+      <c r="J21" s="378"/>
+      <c r="K21" s="378"/>
+      <c r="L21" s="379"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="386" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="505">
+      <c r="C22" s="496">
         <f>BD!B6</f>
         <v>0</v>
       </c>
-      <c r="D22" s="505"/>
-      <c r="E22" s="505"/>
-      <c r="F22" s="505"/>
-      <c r="G22" s="505"/>
-      <c r="H22" s="505"/>
-      <c r="I22" s="505"/>
-      <c r="J22" s="505"/>
-      <c r="K22" s="505"/>
-      <c r="L22" s="451"/>
-    </row>
-    <row r="23" spans="2:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="388" t="s">
+      <c r="D22" s="496"/>
+      <c r="E22" s="496"/>
+      <c r="F22" s="496"/>
+      <c r="G22" s="496"/>
+      <c r="H22" s="496"/>
+      <c r="I22" s="496"/>
+      <c r="J22" s="496"/>
+      <c r="K22" s="496"/>
+      <c r="L22" s="445"/>
+    </row>
+    <row r="23" spans="2:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="387" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="506" t="str">
+      <c r="C23" s="497" t="str">
         <f>"Esta actualización de la Orden de Servicio, tiene como objetivo ajustar el alcance, valor y plazo de la Orden "&amp;F5&amp;" incorporando el alcance de servicio denominado "&amp;F8&amp;" "&amp;BD!B13</f>
         <v xml:space="preserve">Esta actualización de la Orden de Servicio, tiene como objetivo ajustar el alcance, valor y plazo de la Orden  incorporando el alcance de servicio denominado  </v>
       </c>
-      <c r="D23" s="506"/>
-      <c r="E23" s="506"/>
-      <c r="F23" s="506"/>
-      <c r="G23" s="506"/>
-      <c r="H23" s="506"/>
-      <c r="I23" s="506"/>
-      <c r="J23" s="506"/>
-      <c r="K23" s="506"/>
-      <c r="L23" s="394"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="372"/>
+      <c r="D23" s="497"/>
+      <c r="E23" s="497"/>
+      <c r="F23" s="497"/>
+      <c r="G23" s="497"/>
+      <c r="H23" s="497"/>
+      <c r="I23" s="497"/>
+      <c r="J23" s="497"/>
+      <c r="K23" s="497"/>
+      <c r="L23" s="393"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="371"/>
       <c r="C24" s="316"/>
       <c r="D24" s="316"/>
       <c r="E24" s="301"/>
@@ -5729,463 +5736,463 @@
       <c r="H24" s="298"/>
       <c r="I24" s="298"/>
       <c r="J24" s="299"/>
-      <c r="K24" s="425" t="s">
+      <c r="K24" s="419" t="s">
         <v>30</v>
       </c>
-      <c r="L24" s="389">
+      <c r="L24" s="388">
         <f>BD!B18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="390" t="s">
+    <row r="25" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="389" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="412" t="s">
+      <c r="C25" s="407" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="412" t="s">
+      <c r="D25" s="407" t="s">
         <v>154</v>
       </c>
-      <c r="E25" s="410"/>
-      <c r="F25" s="410"/>
-      <c r="G25" s="410"/>
-      <c r="H25" s="411"/>
-      <c r="I25" s="381" t="s">
+      <c r="E25" s="405"/>
+      <c r="F25" s="405"/>
+      <c r="G25" s="405"/>
+      <c r="H25" s="406"/>
+      <c r="I25" s="380" t="s">
         <v>23</v>
       </c>
-      <c r="J25" s="382" t="s">
+      <c r="J25" s="381" t="s">
         <v>155</v>
       </c>
-      <c r="K25" s="383" t="s">
+      <c r="K25" s="382" t="s">
         <v>24</v>
       </c>
-      <c r="L25" s="426" t="s">
+      <c r="L25" s="420" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="391">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="390">
         <f>BD!A31</f>
         <v>0</v>
       </c>
-      <c r="C26" s="408">
+      <c r="C26" s="403">
         <f>BD!B31</f>
         <v>0</v>
       </c>
-      <c r="D26" s="408">
+      <c r="D26" s="403">
         <f>BD!C31</f>
         <v>0</v>
       </c>
-      <c r="E26" s="409"/>
-      <c r="F26" s="409"/>
-      <c r="G26" s="409"/>
-      <c r="H26" s="409"/>
-      <c r="I26" s="384">
+      <c r="E26" s="404"/>
+      <c r="F26" s="404"/>
+      <c r="G26" s="404"/>
+      <c r="H26" s="404"/>
+      <c r="I26" s="383">
         <f>BD!D31</f>
         <v>0</v>
       </c>
-      <c r="J26" s="385">
+      <c r="J26" s="384">
         <f>BD!F31</f>
         <v>0</v>
       </c>
-      <c r="K26" s="386">
+      <c r="K26" s="385">
         <f>BD!E31</f>
         <v>0</v>
       </c>
-      <c r="L26" s="454">
+      <c r="L26" s="448">
         <f>BD!G31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="391">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="390">
         <f>BD!A32</f>
         <v>0</v>
       </c>
-      <c r="C27" s="408">
+      <c r="C27" s="403">
         <f>BD!B32</f>
         <v>0</v>
       </c>
-      <c r="D27" s="408">
+      <c r="D27" s="403">
         <f>BD!C32</f>
         <v>0</v>
       </c>
-      <c r="E27" s="409"/>
-      <c r="F27" s="409"/>
-      <c r="G27" s="409"/>
-      <c r="H27" s="409"/>
-      <c r="I27" s="384">
+      <c r="E27" s="404"/>
+      <c r="F27" s="404"/>
+      <c r="G27" s="404"/>
+      <c r="H27" s="404"/>
+      <c r="I27" s="383">
         <f>BD!D32</f>
         <v>0</v>
       </c>
-      <c r="J27" s="385">
+      <c r="J27" s="384">
         <f>BD!F32</f>
         <v>0</v>
       </c>
-      <c r="K27" s="386">
+      <c r="K27" s="385">
         <f>BD!E32</f>
         <v>0</v>
       </c>
-      <c r="L27" s="454">
+      <c r="L27" s="448">
         <f>BD!G32</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="391">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="390">
         <f>BD!A33</f>
         <v>0</v>
       </c>
-      <c r="C28" s="408">
+      <c r="C28" s="403">
         <f>BD!B33</f>
         <v>0</v>
       </c>
-      <c r="D28" s="408">
+      <c r="D28" s="403">
         <f>BD!C33</f>
         <v>0</v>
       </c>
-      <c r="E28" s="409"/>
-      <c r="F28" s="409"/>
-      <c r="G28" s="409"/>
-      <c r="H28" s="409"/>
-      <c r="I28" s="384">
+      <c r="E28" s="404"/>
+      <c r="F28" s="404"/>
+      <c r="G28" s="404"/>
+      <c r="H28" s="404"/>
+      <c r="I28" s="383">
         <f>BD!D33</f>
         <v>0</v>
       </c>
-      <c r="J28" s="385">
+      <c r="J28" s="384">
         <f>BD!F33</f>
         <v>0</v>
       </c>
-      <c r="K28" s="386">
+      <c r="K28" s="385">
         <f>BD!E33</f>
         <v>0</v>
       </c>
-      <c r="L28" s="454">
+      <c r="L28" s="448">
         <f>BD!G33</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="391">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="390">
         <f>BD!A34</f>
         <v>0</v>
       </c>
-      <c r="C29" s="408">
+      <c r="C29" s="403">
         <f>BD!B34</f>
         <v>0</v>
       </c>
-      <c r="D29" s="408">
+      <c r="D29" s="403">
         <f>BD!C34</f>
         <v>0</v>
       </c>
-      <c r="E29" s="409"/>
-      <c r="F29" s="409"/>
-      <c r="G29" s="409"/>
-      <c r="H29" s="409"/>
-      <c r="I29" s="384">
+      <c r="E29" s="404"/>
+      <c r="F29" s="404"/>
+      <c r="G29" s="404"/>
+      <c r="H29" s="404"/>
+      <c r="I29" s="383">
         <f>BD!D34</f>
         <v>0</v>
       </c>
-      <c r="J29" s="385">
+      <c r="J29" s="384">
         <f>BD!F34</f>
         <v>0</v>
       </c>
-      <c r="K29" s="386">
+      <c r="K29" s="385">
         <f>BD!E34</f>
         <v>0</v>
       </c>
-      <c r="L29" s="454">
+      <c r="L29" s="448">
         <f>BD!G34</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="391">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="390">
         <f>BD!A35</f>
         <v>0</v>
       </c>
-      <c r="C30" s="408">
+      <c r="C30" s="403">
         <f>BD!B35</f>
         <v>0</v>
       </c>
-      <c r="D30" s="408">
+      <c r="D30" s="403">
         <f>BD!C35</f>
         <v>0</v>
       </c>
-      <c r="E30" s="409"/>
-      <c r="F30" s="409"/>
-      <c r="G30" s="409"/>
-      <c r="H30" s="409"/>
-      <c r="I30" s="384">
+      <c r="E30" s="404"/>
+      <c r="F30" s="404"/>
+      <c r="G30" s="404"/>
+      <c r="H30" s="404"/>
+      <c r="I30" s="383">
         <f>BD!D35</f>
         <v>0</v>
       </c>
-      <c r="J30" s="385">
+      <c r="J30" s="384">
         <f>BD!F35</f>
         <v>0</v>
       </c>
-      <c r="K30" s="386">
+      <c r="K30" s="385">
         <f>BD!E35</f>
         <v>0</v>
       </c>
-      <c r="L30" s="454">
+      <c r="L30" s="448">
         <f>BD!G35</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="391">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="390">
         <f>BD!A36</f>
         <v>0</v>
       </c>
-      <c r="C31" s="408">
+      <c r="C31" s="403">
         <f>BD!B36</f>
         <v>0</v>
       </c>
-      <c r="D31" s="408">
+      <c r="D31" s="403">
         <f>BD!C36</f>
         <v>0</v>
       </c>
-      <c r="E31" s="409"/>
-      <c r="F31" s="409"/>
-      <c r="G31" s="409"/>
-      <c r="H31" s="409"/>
-      <c r="I31" s="384">
+      <c r="E31" s="404"/>
+      <c r="F31" s="404"/>
+      <c r="G31" s="404"/>
+      <c r="H31" s="404"/>
+      <c r="I31" s="383">
         <f>BD!D36</f>
         <v>0</v>
       </c>
-      <c r="J31" s="385">
+      <c r="J31" s="384">
         <f>BD!F36</f>
         <v>0</v>
       </c>
-      <c r="K31" s="386">
+      <c r="K31" s="385">
         <f>BD!E36</f>
         <v>0</v>
       </c>
-      <c r="L31" s="454">
+      <c r="L31" s="448">
         <f>BD!G36</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="391">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="390">
         <f>BD!A37</f>
         <v>0</v>
       </c>
-      <c r="C32" s="408">
+      <c r="C32" s="403">
         <f>BD!B37</f>
         <v>0</v>
       </c>
-      <c r="D32" s="408">
+      <c r="D32" s="403">
         <f>BD!C37</f>
         <v>0</v>
       </c>
-      <c r="E32" s="409"/>
-      <c r="F32" s="409"/>
-      <c r="G32" s="409"/>
-      <c r="H32" s="409"/>
-      <c r="I32" s="384">
+      <c r="E32" s="404"/>
+      <c r="F32" s="404"/>
+      <c r="G32" s="404"/>
+      <c r="H32" s="404"/>
+      <c r="I32" s="383">
         <f>BD!D37</f>
         <v>0</v>
       </c>
-      <c r="J32" s="385">
+      <c r="J32" s="384">
         <f>BD!F37</f>
         <v>0</v>
       </c>
-      <c r="K32" s="386">
+      <c r="K32" s="385">
         <f>BD!E37</f>
         <v>0</v>
       </c>
-      <c r="L32" s="454">
+      <c r="L32" s="448">
         <f>BD!G37</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B33" s="391">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="390">
         <f>BD!A38</f>
         <v>0</v>
       </c>
-      <c r="C33" s="408">
+      <c r="C33" s="403">
         <f>BD!B38</f>
         <v>0</v>
       </c>
-      <c r="D33" s="408">
+      <c r="D33" s="403">
         <f>BD!C38</f>
         <v>0</v>
       </c>
-      <c r="E33" s="409"/>
-      <c r="F33" s="409"/>
-      <c r="G33" s="409"/>
-      <c r="H33" s="409"/>
-      <c r="I33" s="384">
+      <c r="E33" s="404"/>
+      <c r="F33" s="404"/>
+      <c r="G33" s="404"/>
+      <c r="H33" s="404"/>
+      <c r="I33" s="383">
         <f>BD!D38</f>
         <v>0</v>
       </c>
-      <c r="J33" s="385">
+      <c r="J33" s="384">
         <f>BD!F38</f>
         <v>0</v>
       </c>
-      <c r="K33" s="386">
+      <c r="K33" s="385">
         <f>BD!E38</f>
         <v>0</v>
       </c>
-      <c r="L33" s="454">
+      <c r="L33" s="448">
         <f>BD!G38</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B34" s="391">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="390">
         <f>BD!A39</f>
         <v>0</v>
       </c>
-      <c r="C34" s="408">
+      <c r="C34" s="403">
         <f>BD!B39</f>
         <v>0</v>
       </c>
-      <c r="D34" s="408">
+      <c r="D34" s="403">
         <f>BD!C39</f>
         <v>0</v>
       </c>
-      <c r="E34" s="409"/>
-      <c r="F34" s="409"/>
-      <c r="G34" s="409"/>
-      <c r="H34" s="409"/>
-      <c r="I34" s="384">
+      <c r="E34" s="404"/>
+      <c r="F34" s="404"/>
+      <c r="G34" s="404"/>
+      <c r="H34" s="404"/>
+      <c r="I34" s="383">
         <f>BD!D39</f>
         <v>0</v>
       </c>
-      <c r="J34" s="385">
+      <c r="J34" s="384">
         <f>BD!F39</f>
         <v>0</v>
       </c>
-      <c r="K34" s="386">
+      <c r="K34" s="385">
         <f>BD!E39</f>
         <v>0</v>
       </c>
-      <c r="L34" s="454">
+      <c r="L34" s="448">
         <f>BD!G39</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B35" s="391">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="390">
         <f>BD!A40</f>
         <v>0</v>
       </c>
-      <c r="C35" s="408">
+      <c r="C35" s="403">
         <f>BD!B40</f>
         <v>0</v>
       </c>
-      <c r="D35" s="408">
+      <c r="D35" s="403">
         <f>BD!C40</f>
         <v>0</v>
       </c>
-      <c r="E35" s="409"/>
-      <c r="F35" s="409"/>
-      <c r="G35" s="409"/>
-      <c r="H35" s="409"/>
-      <c r="I35" s="384">
+      <c r="E35" s="404"/>
+      <c r="F35" s="404"/>
+      <c r="G35" s="404"/>
+      <c r="H35" s="404"/>
+      <c r="I35" s="383">
         <f>BD!D40</f>
         <v>0</v>
       </c>
-      <c r="J35" s="385">
+      <c r="J35" s="384">
         <f>BD!F40</f>
         <v>0</v>
       </c>
-      <c r="K35" s="386">
+      <c r="K35" s="385">
         <f>BD!E40</f>
         <v>0</v>
       </c>
-      <c r="L35" s="454">
+      <c r="L35" s="448">
         <f>BD!G40</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B36" s="391">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="390">
         <f>BD!A41</f>
         <v>0</v>
       </c>
-      <c r="C36" s="408">
+      <c r="C36" s="403">
         <f>BD!B41</f>
         <v>0</v>
       </c>
-      <c r="D36" s="408">
+      <c r="D36" s="403">
         <f>BD!C41</f>
         <v>0</v>
       </c>
-      <c r="E36" s="409"/>
-      <c r="F36" s="409"/>
-      <c r="G36" s="409"/>
-      <c r="H36" s="409"/>
-      <c r="I36" s="384">
+      <c r="E36" s="404"/>
+      <c r="F36" s="404"/>
+      <c r="G36" s="404"/>
+      <c r="H36" s="404"/>
+      <c r="I36" s="383">
         <f>BD!D41</f>
         <v>0</v>
       </c>
-      <c r="J36" s="385">
+      <c r="J36" s="384">
         <f>BD!F41</f>
         <v>0</v>
       </c>
-      <c r="K36" s="386">
+      <c r="K36" s="385">
         <f>BD!E41</f>
         <v>0</v>
       </c>
-      <c r="L36" s="454">
+      <c r="L36" s="448">
         <f>BD!G41</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B37" s="391">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="390">
         <f>BD!A42</f>
         <v>0</v>
       </c>
-      <c r="C37" s="408">
+      <c r="C37" s="403">
         <f>BD!B42</f>
         <v>0</v>
       </c>
-      <c r="D37" s="408">
+      <c r="D37" s="403">
         <f>BD!C42</f>
         <v>0</v>
       </c>
-      <c r="E37" s="409"/>
-      <c r="F37" s="409"/>
-      <c r="G37" s="409"/>
-      <c r="H37" s="409"/>
-      <c r="I37" s="384">
+      <c r="E37" s="404"/>
+      <c r="F37" s="404"/>
+      <c r="G37" s="404"/>
+      <c r="H37" s="404"/>
+      <c r="I37" s="383">
         <f>BD!D42</f>
         <v>0</v>
       </c>
-      <c r="J37" s="385">
+      <c r="J37" s="384">
         <f>BD!F42</f>
         <v>0</v>
       </c>
-      <c r="K37" s="386">
+      <c r="K37" s="385">
         <f>BD!E42</f>
         <v>0</v>
       </c>
-      <c r="L37" s="454">
+      <c r="L37" s="448">
         <f>BD!G42</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="413"/>
-      <c r="C38" s="358"/>
-      <c r="D38" s="358"/>
-      <c r="E38" s="358"/>
-      <c r="F38" s="358"/>
-      <c r="G38" s="358"/>
-      <c r="H38" s="358"/>
-      <c r="I38" s="358"/>
-      <c r="J38" s="358"/>
-      <c r="K38" s="358"/>
-      <c r="L38" s="455"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="408"/>
+      <c r="C38" s="357"/>
+      <c r="D38" s="357"/>
+      <c r="E38" s="357"/>
+      <c r="F38" s="357"/>
+      <c r="G38" s="357"/>
+      <c r="H38" s="357"/>
+      <c r="I38" s="357"/>
+      <c r="J38" s="357"/>
+      <c r="K38" s="357"/>
+      <c r="L38" s="449"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="321" t="s">
         <v>157</v>
       </c>
@@ -6195,53 +6202,54 @@
       <c r="F39" s="322"/>
       <c r="G39" s="322"/>
       <c r="H39" s="323"/>
-      <c r="I39" s="493" t="s">
+      <c r="I39" s="491" t="str">
+        <f>"Valor Neto ("&amp;BD!B18&amp;" ) :"</f>
+        <v>Valor Neto ( ) :</v>
+      </c>
+      <c r="J39" s="492"/>
+      <c r="K39" s="493"/>
+      <c r="L39" s="450">
+        <f>SUM(L26:L37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="494" t="s">
         <v>158</v>
       </c>
-      <c r="J39" s="494"/>
-      <c r="K39" s="495"/>
-      <c r="L39" s="456">
-        <f>SUM(L26:L37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="496" t="s">
+      <c r="C40" s="495"/>
+      <c r="D40" s="495"/>
+      <c r="E40" s="495"/>
+      <c r="F40" s="495"/>
+      <c r="G40" s="495"/>
+      <c r="H40" s="418"/>
+      <c r="I40" s="491" t="s">
         <v>159</v>
       </c>
-      <c r="C40" s="497"/>
-      <c r="D40" s="497"/>
-      <c r="E40" s="497"/>
-      <c r="F40" s="497"/>
-      <c r="G40" s="497"/>
-      <c r="H40" s="424"/>
-      <c r="I40" s="493" t="s">
+      <c r="J40" s="492"/>
+      <c r="K40" s="493"/>
+      <c r="L40" s="451"/>
+    </row>
+    <row r="41" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="494"/>
+      <c r="C41" s="495"/>
+      <c r="D41" s="495"/>
+      <c r="E41" s="495"/>
+      <c r="F41" s="495"/>
+      <c r="G41" s="495"/>
+      <c r="H41" s="418"/>
+      <c r="I41" s="491" t="s">
         <v>160</v>
       </c>
-      <c r="J40" s="494"/>
-      <c r="K40" s="495"/>
-      <c r="L40" s="457"/>
-    </row>
-    <row r="41" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="496"/>
-      <c r="C41" s="497"/>
-      <c r="D41" s="497"/>
-      <c r="E41" s="497"/>
-      <c r="F41" s="497"/>
-      <c r="G41" s="497"/>
-      <c r="H41" s="424"/>
-      <c r="I41" s="493" t="s">
+      <c r="J41" s="492"/>
+      <c r="K41" s="493"/>
+      <c r="L41" s="450">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="324" t="s">
         <v>161</v>
-      </c>
-      <c r="J41" s="494"/>
-      <c r="K41" s="495"/>
-      <c r="L41" s="456">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="324" t="s">
-        <v>162</v>
       </c>
       <c r="C42" s="325"/>
       <c r="D42" s="325"/>
@@ -6249,34 +6257,36 @@
       <c r="F42" s="325"/>
       <c r="G42" s="325"/>
       <c r="H42" s="326"/>
-      <c r="I42" s="427"/>
-      <c r="J42" s="428"/>
-      <c r="K42" s="329" t="s">
-        <v>163</v>
-      </c>
-      <c r="L42" s="458">
+      <c r="I42" s="421"/>
+      <c r="J42" s="422"/>
+      <c r="K42" s="329" t="str">
+        <f>"TOTAL ACTUALIZACIÓN ("&amp;BD!B18&amp;" ) :"</f>
+        <v>TOTAL ACTUALIZACIÓN ( ) :</v>
+      </c>
+      <c r="L42" s="452">
         <f>L38</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B43" s="479"/>
-      <c r="C43" s="480"/>
-      <c r="D43" s="480"/>
-      <c r="E43" s="480"/>
-      <c r="F43" s="480"/>
-      <c r="G43" s="480"/>
-      <c r="H43" s="481"/>
-      <c r="I43" s="452" t="s">
-        <v>164</v>
-      </c>
-      <c r="J43" s="453"/>
-      <c r="K43" s="447"/>
-      <c r="L43" s="459"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B44" s="392" t="s">
-        <v>165</v>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="473"/>
+      <c r="C43" s="474"/>
+      <c r="D43" s="474"/>
+      <c r="E43" s="474"/>
+      <c r="F43" s="474"/>
+      <c r="G43" s="474"/>
+      <c r="H43" s="475"/>
+      <c r="I43" s="446" t="str">
+        <f>"TOTAL ORDEN DE SERVICIO EN " &amp;BD!B18</f>
+        <v xml:space="preserve">TOTAL ORDEN DE SERVICIO EN </v>
+      </c>
+      <c r="J43" s="447"/>
+      <c r="K43" s="441"/>
+      <c r="L43" s="453"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="391" t="s">
+        <v>162</v>
       </c>
       <c r="C44" s="316"/>
       <c r="D44" s="210"/>
@@ -6284,82 +6294,84 @@
       <c r="F44" s="210"/>
       <c r="G44" s="210"/>
       <c r="H44" s="328"/>
-      <c r="I44" s="432"/>
-      <c r="J44" s="419"/>
-      <c r="K44" s="418" t="s">
-        <v>166</v>
-      </c>
-      <c r="L44" s="456">
+      <c r="I44" s="482"/>
+      <c r="J44" s="413"/>
+      <c r="K44" s="483" t="str">
+        <f>"MONTO INICIAL "&amp;BD!B5&amp;" :"</f>
+        <v>MONTO INICIAL  :</v>
+      </c>
+      <c r="L44" s="450">
         <f>BD!B19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="432"/>
-      <c r="C45" s="462"/>
+    <row r="45" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="426"/>
+      <c r="C45" s="456"/>
       <c r="D45" s="327"/>
       <c r="E45" s="327"/>
       <c r="F45" s="327"/>
       <c r="G45" s="327"/>
       <c r="H45" s="306"/>
-      <c r="I45" s="432"/>
-      <c r="J45" s="419"/>
-      <c r="K45" s="418" t="s">
-        <v>204</v>
-      </c>
-      <c r="L45" s="456">
+      <c r="I45" s="482"/>
+      <c r="J45" s="413"/>
+      <c r="K45" s="483" t="s">
+        <v>200</v>
+      </c>
+      <c r="L45" s="450">
         <f>BD!B20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B46" s="507" t="s">
-        <v>167</v>
-      </c>
-      <c r="C46" s="508"/>
-      <c r="D46" s="395">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="498" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="499"/>
+      <c r="D46" s="394">
         <f>BD!B22</f>
         <v>0</v>
       </c>
-      <c r="E46" s="461" t="s">
-        <v>168</v>
-      </c>
-      <c r="F46" s="509">
+      <c r="E46" s="455" t="s">
+        <v>164</v>
+      </c>
+      <c r="F46" s="500">
         <f>BD!B25</f>
         <v>0</v>
       </c>
-      <c r="G46" s="509"/>
+      <c r="G46" s="500"/>
       <c r="H46" s="210"/>
-      <c r="I46" s="432"/>
-      <c r="J46" s="419"/>
-      <c r="K46" s="418" t="s">
-        <v>205</v>
-      </c>
-      <c r="L46" s="456">
+      <c r="I46" s="484"/>
+      <c r="J46" s="413"/>
+      <c r="K46" s="483" t="s">
+        <v>201</v>
+      </c>
+      <c r="L46" s="450">
         <f>BD!B21</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="432"/>
+    <row r="47" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="426"/>
       <c r="C47" s="210"/>
       <c r="D47" s="210"/>
       <c r="E47" s="210"/>
       <c r="F47" s="210"/>
       <c r="G47" s="210"/>
       <c r="H47" s="210"/>
-      <c r="I47" s="449"/>
-      <c r="J47" s="421"/>
-      <c r="K47" s="420" t="s">
-        <v>207</v>
-      </c>
-      <c r="L47" s="458">
+      <c r="I47" s="443"/>
+      <c r="J47" s="415"/>
+      <c r="K47" s="414" t="str">
+        <f>"TOTAL ACUM NETO "&amp;BD!B5</f>
+        <v xml:space="preserve">TOTAL ACUM NETO </v>
+      </c>
+      <c r="L47" s="452">
         <f>L44+L45+L46</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="432"/>
+    <row r="48" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="426"/>
       <c r="C48" s="210"/>
       <c r="D48" s="210"/>
       <c r="E48" s="210"/>
@@ -6369,387 +6381,387 @@
       <c r="I48" s="330"/>
       <c r="J48" s="331"/>
       <c r="K48" s="332"/>
-      <c r="L48" s="393"/>
-    </row>
-    <row r="49" spans="2:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="449"/>
-      <c r="C49" s="422"/>
-      <c r="D49" s="422"/>
-      <c r="E49" s="422"/>
-      <c r="F49" s="422"/>
-      <c r="G49" s="422"/>
-      <c r="H49" s="422"/>
-      <c r="I49" s="422"/>
-      <c r="J49" s="422"/>
-      <c r="K49" s="422"/>
-      <c r="L49" s="423"/>
-    </row>
-    <row r="50" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="470" t="s">
+      <c r="L48" s="392"/>
+    </row>
+    <row r="49" spans="2:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="443"/>
+      <c r="C49" s="416"/>
+      <c r="D49" s="416"/>
+      <c r="E49" s="416"/>
+      <c r="F49" s="416"/>
+      <c r="G49" s="416"/>
+      <c r="H49" s="416"/>
+      <c r="I49" s="416"/>
+      <c r="J49" s="416"/>
+      <c r="K49" s="416"/>
+      <c r="L49" s="417"/>
+    </row>
+    <row r="50" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="464" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50" s="465"/>
+      <c r="D50" s="466"/>
+      <c r="E50" s="466"/>
+      <c r="F50" s="467"/>
+      <c r="G50" s="514" t="s">
+        <v>166</v>
+      </c>
+      <c r="H50" s="514"/>
+      <c r="I50" s="514"/>
+      <c r="J50" s="514"/>
+      <c r="K50" s="514"/>
+      <c r="L50" s="468"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="519" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" s="395" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="395">
+        <v>0</v>
+      </c>
+      <c r="E51" s="520"/>
+      <c r="F51" s="333"/>
+      <c r="G51" s="515"/>
+      <c r="H51" s="515"/>
+      <c r="I51" s="515"/>
+      <c r="J51" s="515"/>
+      <c r="K51" s="515"/>
+      <c r="L51" s="427"/>
+    </row>
+    <row r="52" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="521" t="s">
+        <v>168</v>
+      </c>
+      <c r="C52" s="522"/>
+      <c r="D52" s="523" t="s">
         <v>169</v>
       </c>
-      <c r="C50" s="471"/>
-      <c r="D50" s="472"/>
-      <c r="E50" s="472"/>
-      <c r="F50" s="473"/>
-      <c r="G50" s="502" t="s">
+      <c r="E52" s="524"/>
+      <c r="F52" s="454"/>
+      <c r="G52" s="515"/>
+      <c r="H52" s="515"/>
+      <c r="I52" s="515"/>
+      <c r="J52" s="515"/>
+      <c r="K52" s="515"/>
+      <c r="L52" s="427"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="519" t="s">
         <v>170</v>
       </c>
-      <c r="H50" s="502"/>
-      <c r="I50" s="502"/>
-      <c r="J50" s="502"/>
-      <c r="K50" s="502"/>
-      <c r="L50" s="474"/>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B51" s="434" t="s">
+      <c r="C53" s="525" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" s="526"/>
+      <c r="E53" s="526"/>
+      <c r="F53" s="454"/>
+      <c r="G53" s="515"/>
+      <c r="H53" s="515"/>
+      <c r="I53" s="515"/>
+      <c r="J53" s="515"/>
+      <c r="K53" s="515"/>
+      <c r="L53" s="427"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="428" t="s">
         <v>171</v>
       </c>
-      <c r="C51" s="396" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" s="396">
-        <v>0</v>
-      </c>
-      <c r="E51" s="333"/>
-      <c r="F51" s="334"/>
-      <c r="G51" s="503"/>
-      <c r="H51" s="503"/>
-      <c r="I51" s="503"/>
-      <c r="J51" s="503"/>
-      <c r="K51" s="503"/>
-      <c r="L51" s="433"/>
-    </row>
-    <row r="52" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="498" t="s">
+      <c r="C54" s="334"/>
+      <c r="D54" s="334"/>
+      <c r="E54" s="335"/>
+      <c r="F54" s="336"/>
+      <c r="G54" s="515"/>
+      <c r="H54" s="515"/>
+      <c r="I54" s="515"/>
+      <c r="J54" s="515"/>
+      <c r="K54" s="515"/>
+      <c r="L54" s="427"/>
+    </row>
+    <row r="55" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="517" t="s">
         <v>172</v>
       </c>
-      <c r="C52" s="499"/>
-      <c r="D52" s="399" t="s">
+      <c r="C55" s="518"/>
+      <c r="D55" s="518"/>
+      <c r="E55" s="518"/>
+      <c r="F55" s="410"/>
+      <c r="G55" s="515"/>
+      <c r="H55" s="515"/>
+      <c r="I55" s="515"/>
+      <c r="J55" s="515"/>
+      <c r="K55" s="515"/>
+      <c r="L55" s="427"/>
+    </row>
+    <row r="56" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="517"/>
+      <c r="C56" s="518"/>
+      <c r="D56" s="518"/>
+      <c r="E56" s="518"/>
+      <c r="F56" s="410"/>
+      <c r="G56" s="515"/>
+      <c r="H56" s="515"/>
+      <c r="I56" s="515"/>
+      <c r="J56" s="515"/>
+      <c r="K56" s="515"/>
+      <c r="L56" s="427"/>
+    </row>
+    <row r="57" spans="2:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="429"/>
+      <c r="C57" s="411"/>
+      <c r="D57" s="411"/>
+      <c r="E57" s="411"/>
+      <c r="F57" s="411"/>
+      <c r="G57" s="516" t="s">
         <v>173</v>
       </c>
-      <c r="E52" s="400"/>
-      <c r="F52" s="460"/>
-      <c r="G52" s="503"/>
-      <c r="H52" s="503"/>
-      <c r="I52" s="503"/>
-      <c r="J52" s="503"/>
-      <c r="K52" s="503"/>
-      <c r="L52" s="433"/>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B53" s="434" t="s">
-        <v>174</v>
-      </c>
-      <c r="C53" s="397" t="s">
-        <v>85</v>
-      </c>
-      <c r="D53" s="398"/>
-      <c r="E53" s="398"/>
-      <c r="F53" s="460"/>
-      <c r="G53" s="503"/>
-      <c r="H53" s="503"/>
-      <c r="I53" s="503"/>
-      <c r="J53" s="503"/>
-      <c r="K53" s="503"/>
-      <c r="L53" s="433"/>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B54" s="434" t="s">
-        <v>175</v>
-      </c>
-      <c r="C54" s="335"/>
-      <c r="D54" s="335"/>
-      <c r="E54" s="336"/>
-      <c r="F54" s="337"/>
-      <c r="G54" s="503"/>
-      <c r="H54" s="503"/>
-      <c r="I54" s="503"/>
-      <c r="J54" s="503"/>
-      <c r="K54" s="503"/>
-      <c r="L54" s="433"/>
-    </row>
-    <row r="55" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="500" t="s">
-        <v>176</v>
-      </c>
-      <c r="C55" s="501"/>
-      <c r="D55" s="501"/>
-      <c r="E55" s="501"/>
-      <c r="F55" s="415"/>
-      <c r="G55" s="503"/>
-      <c r="H55" s="503"/>
-      <c r="I55" s="503"/>
-      <c r="J55" s="503"/>
-      <c r="K55" s="503"/>
-      <c r="L55" s="433"/>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B56" s="500"/>
-      <c r="C56" s="501"/>
-      <c r="D56" s="501"/>
-      <c r="E56" s="501"/>
-      <c r="F56" s="415"/>
-      <c r="G56" s="503"/>
-      <c r="H56" s="503"/>
-      <c r="I56" s="503"/>
-      <c r="J56" s="503"/>
-      <c r="K56" s="503"/>
-      <c r="L56" s="433"/>
-    </row>
-    <row r="57" spans="2:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="435"/>
-      <c r="C57" s="416"/>
-      <c r="D57" s="416"/>
-      <c r="E57" s="416"/>
-      <c r="F57" s="416"/>
-      <c r="G57" s="504" t="s">
-        <v>177</v>
-      </c>
-      <c r="H57" s="504"/>
-      <c r="I57" s="504"/>
-      <c r="J57" s="504"/>
-      <c r="K57" s="504"/>
-      <c r="L57" s="436"/>
-    </row>
-    <row r="58" spans="2:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="475"/>
-      <c r="C58" s="476"/>
-      <c r="D58" s="476"/>
-      <c r="E58" s="476"/>
-      <c r="F58" s="476"/>
-      <c r="G58" s="476"/>
-      <c r="H58" s="477"/>
-      <c r="I58" s="477"/>
-      <c r="J58" s="477"/>
-      <c r="K58" s="477"/>
-      <c r="L58" s="478"/>
-    </row>
-    <row r="59" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="450"/>
-      <c r="C59" s="417"/>
-      <c r="D59" s="417"/>
-      <c r="E59" s="438"/>
-      <c r="F59" s="437" t="str">
+      <c r="H57" s="516"/>
+      <c r="I57" s="516"/>
+      <c r="J57" s="516"/>
+      <c r="K57" s="516"/>
+      <c r="L57" s="430"/>
+    </row>
+    <row r="58" spans="2:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="469"/>
+      <c r="C58" s="470"/>
+      <c r="D58" s="470"/>
+      <c r="E58" s="470"/>
+      <c r="F58" s="470"/>
+      <c r="G58" s="470"/>
+      <c r="H58" s="471"/>
+      <c r="I58" s="471"/>
+      <c r="J58" s="471"/>
+      <c r="K58" s="471"/>
+      <c r="L58" s="472"/>
+    </row>
+    <row r="59" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="444"/>
+      <c r="C59" s="412"/>
+      <c r="D59" s="412"/>
+      <c r="E59" s="432"/>
+      <c r="F59" s="431" t="str">
         <f>"Aprobaciones "&amp;BD!B29</f>
         <v xml:space="preserve">Aprobaciones </v>
       </c>
-      <c r="G59" s="437"/>
-      <c r="H59" s="417"/>
-      <c r="I59" s="417"/>
-      <c r="J59" s="417"/>
-      <c r="K59" s="417"/>
-      <c r="L59" s="438"/>
-    </row>
-    <row r="60" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="465"/>
-      <c r="C60" s="466"/>
-      <c r="D60" s="467"/>
-      <c r="E60" s="467"/>
-      <c r="F60" s="468"/>
-      <c r="G60" s="468"/>
-      <c r="H60" s="468"/>
-      <c r="I60" s="468"/>
-      <c r="J60" s="468"/>
-      <c r="K60" s="468"/>
-      <c r="L60" s="365"/>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B61" s="432"/>
-      <c r="C61" s="339" t="s">
-        <v>179</v>
-      </c>
-      <c r="D61" s="339"/>
-      <c r="E61" s="340"/>
-      <c r="F61" s="340"/>
+      <c r="G59" s="431"/>
+      <c r="H59" s="412"/>
+      <c r="I59" s="412"/>
+      <c r="J59" s="412"/>
+      <c r="K59" s="412"/>
+      <c r="L59" s="432"/>
+    </row>
+    <row r="60" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="459"/>
+      <c r="C60" s="460"/>
+      <c r="D60" s="461"/>
+      <c r="E60" s="461"/>
+      <c r="F60" s="462"/>
+      <c r="G60" s="462"/>
+      <c r="H60" s="462"/>
+      <c r="I60" s="462"/>
+      <c r="J60" s="462"/>
+      <c r="K60" s="462"/>
+      <c r="L60" s="364"/>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B61" s="426"/>
+      <c r="C61" s="338" t="s">
+        <v>175</v>
+      </c>
+      <c r="D61" s="338"/>
+      <c r="E61" s="339"/>
+      <c r="F61" s="339"/>
       <c r="G61" s="307"/>
-      <c r="H61" s="462"/>
-      <c r="I61" s="339" t="s">
-        <v>179</v>
-      </c>
-      <c r="J61" s="341"/>
-      <c r="K61" s="341"/>
-      <c r="L61" s="368"/>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B62" s="432"/>
-      <c r="C62" s="343" t="s">
+      <c r="H61" s="456"/>
+      <c r="I61" s="338" t="s">
+        <v>175</v>
+      </c>
+      <c r="J61" s="340"/>
+      <c r="K61" s="340"/>
+      <c r="L61" s="367"/>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B62" s="426"/>
+      <c r="C62" s="342" t="s">
         <v>112</v>
       </c>
-      <c r="D62" s="343"/>
-      <c r="E62" s="343"/>
-      <c r="F62" s="343"/>
-      <c r="G62" s="344"/>
-      <c r="H62" s="462"/>
-      <c r="I62" s="343" t="s">
-        <v>180</v>
-      </c>
-      <c r="J62" s="345"/>
-      <c r="K62" s="345"/>
-      <c r="L62" s="440"/>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B63" s="432"/>
-      <c r="C63" s="343" t="s">
+      <c r="D62" s="342"/>
+      <c r="E62" s="342"/>
+      <c r="F62" s="342"/>
+      <c r="G62" s="343"/>
+      <c r="H62" s="456"/>
+      <c r="I62" s="342" t="s">
+        <v>176</v>
+      </c>
+      <c r="J62" s="344"/>
+      <c r="K62" s="344"/>
+      <c r="L62" s="434"/>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B63" s="426"/>
+      <c r="C63" s="342" t="s">
         <v>114</v>
       </c>
-      <c r="D63" s="343"/>
-      <c r="E63" s="343"/>
-      <c r="F63" s="343"/>
-      <c r="G63" s="344"/>
-      <c r="H63" s="462"/>
-      <c r="I63" s="343" t="s">
-        <v>181</v>
-      </c>
-      <c r="J63" s="346"/>
-      <c r="K63" s="346"/>
-      <c r="L63" s="440"/>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B64" s="432"/>
+      <c r="D63" s="342"/>
+      <c r="E63" s="342"/>
+      <c r="F63" s="342"/>
+      <c r="G63" s="343"/>
+      <c r="H63" s="456"/>
+      <c r="I63" s="342" t="s">
+        <v>177</v>
+      </c>
+      <c r="J63" s="345"/>
+      <c r="K63" s="345"/>
+      <c r="L63" s="434"/>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B64" s="426"/>
       <c r="C64" s="312"/>
       <c r="D64" s="312"/>
-      <c r="E64" s="347"/>
-      <c r="F64" s="347"/>
+      <c r="E64" s="346"/>
+      <c r="F64" s="346"/>
       <c r="G64" s="307"/>
-      <c r="H64" s="462"/>
+      <c r="H64" s="456"/>
       <c r="I64" s="312"/>
-      <c r="J64" s="341"/>
-      <c r="K64" s="341"/>
-      <c r="L64" s="368"/>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B65" s="432"/>
-      <c r="C65" s="343" t="s">
+      <c r="J64" s="340"/>
+      <c r="K64" s="340"/>
+      <c r="L64" s="367"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="426"/>
+      <c r="C65" s="342" t="s">
         <v>116</v>
       </c>
-      <c r="D65" s="349"/>
-      <c r="E65" s="350"/>
-      <c r="F65" s="346"/>
-      <c r="G65" s="344"/>
-      <c r="H65" s="462"/>
-      <c r="I65" s="343" t="s">
+      <c r="D65" s="348"/>
+      <c r="E65" s="349"/>
+      <c r="F65" s="345"/>
+      <c r="G65" s="343"/>
+      <c r="H65" s="456"/>
+      <c r="I65" s="342" t="s">
         <v>116</v>
       </c>
-      <c r="J65" s="351"/>
-      <c r="K65" s="351"/>
-      <c r="L65" s="368"/>
-    </row>
-    <row r="66" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="441"/>
-      <c r="C66" s="347"/>
-      <c r="D66" s="347"/>
-      <c r="E66" s="352"/>
-      <c r="F66" s="352"/>
+      <c r="J65" s="350"/>
+      <c r="K65" s="350"/>
+      <c r="L65" s="367"/>
+    </row>
+    <row r="66" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="435"/>
+      <c r="C66" s="346"/>
+      <c r="D66" s="346"/>
+      <c r="E66" s="351"/>
+      <c r="F66" s="351"/>
       <c r="G66" s="307"/>
-      <c r="H66" s="347"/>
-      <c r="I66" s="347"/>
-      <c r="J66" s="341"/>
-      <c r="K66" s="341"/>
-      <c r="L66" s="368"/>
-    </row>
-    <row r="67" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="450"/>
-      <c r="C67" s="430"/>
-      <c r="D67" s="430"/>
-      <c r="E67" s="430"/>
-      <c r="F67" s="429" t="str">
+      <c r="H66" s="346"/>
+      <c r="I66" s="346"/>
+      <c r="J66" s="340"/>
+      <c r="K66" s="340"/>
+      <c r="L66" s="367"/>
+    </row>
+    <row r="67" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="444"/>
+      <c r="C67" s="424"/>
+      <c r="D67" s="424"/>
+      <c r="E67" s="424"/>
+      <c r="F67" s="423" t="str">
         <f>"Aceptación de la Actualización "&amp;MID('Orden Cambio'!E8,5,2)&amp;" "&amp;C5&amp; " por "&amp;BD!B7</f>
         <v xml:space="preserve">Aceptación de la Actualización  0 por </v>
       </c>
-      <c r="G67" s="430"/>
-      <c r="H67" s="430"/>
-      <c r="I67" s="430"/>
-      <c r="J67" s="430"/>
-      <c r="K67" s="430"/>
-      <c r="L67" s="431"/>
-    </row>
-    <row r="68" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="439"/>
-      <c r="C68" s="353"/>
-      <c r="D68" s="348"/>
-      <c r="E68" s="339"/>
-      <c r="F68" s="340"/>
-      <c r="G68" s="340"/>
-      <c r="H68" s="342"/>
-      <c r="I68" s="342"/>
-      <c r="J68" s="342"/>
-      <c r="K68" s="342"/>
-      <c r="L68" s="368"/>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B69" s="439" t="s">
-        <v>183</v>
-      </c>
-      <c r="C69" s="357"/>
-      <c r="D69" s="354"/>
-      <c r="E69" s="347"/>
-      <c r="F69" s="347"/>
-      <c r="G69" s="347"/>
-      <c r="H69" s="342"/>
-      <c r="I69" s="342"/>
-      <c r="J69" s="342"/>
-      <c r="K69" s="342"/>
-      <c r="L69" s="368"/>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B70" s="439" t="s">
-        <v>184</v>
-      </c>
-      <c r="C70" s="357"/>
-      <c r="D70" s="354"/>
-      <c r="E70" s="347"/>
-      <c r="F70" s="347"/>
-      <c r="G70" s="347"/>
-      <c r="H70" s="342"/>
-      <c r="I70" s="342"/>
-      <c r="J70" s="342"/>
-      <c r="K70" s="342"/>
-      <c r="L70" s="368"/>
-    </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B71" s="441" t="s">
+      <c r="G67" s="424"/>
+      <c r="H67" s="424"/>
+      <c r="I67" s="424"/>
+      <c r="J67" s="424"/>
+      <c r="K67" s="424"/>
+      <c r="L67" s="425"/>
+    </row>
+    <row r="68" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="433"/>
+      <c r="C68" s="352"/>
+      <c r="D68" s="347"/>
+      <c r="E68" s="338"/>
+      <c r="F68" s="339"/>
+      <c r="G68" s="339"/>
+      <c r="H68" s="341"/>
+      <c r="I68" s="341"/>
+      <c r="J68" s="341"/>
+      <c r="K68" s="341"/>
+      <c r="L68" s="367"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="433" t="s">
+        <v>179</v>
+      </c>
+      <c r="C69" s="356"/>
+      <c r="D69" s="353"/>
+      <c r="E69" s="346"/>
+      <c r="F69" s="346"/>
+      <c r="G69" s="346"/>
+      <c r="H69" s="341"/>
+      <c r="I69" s="341"/>
+      <c r="J69" s="341"/>
+      <c r="K69" s="341"/>
+      <c r="L69" s="367"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B70" s="433" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="356"/>
+      <c r="D70" s="353"/>
+      <c r="E70" s="346"/>
+      <c r="F70" s="346"/>
+      <c r="G70" s="346"/>
+      <c r="H70" s="341"/>
+      <c r="I70" s="341"/>
+      <c r="J70" s="341"/>
+      <c r="K70" s="341"/>
+      <c r="L70" s="367"/>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="435" t="s">
         <v>116</v>
       </c>
       <c r="C71" s="153"/>
       <c r="D71" s="135"/>
-      <c r="E71" s="355"/>
-      <c r="F71" s="355"/>
-      <c r="G71" s="355"/>
-      <c r="H71" s="356"/>
-      <c r="I71" s="342"/>
-      <c r="J71" s="342"/>
-      <c r="K71" s="342"/>
-      <c r="L71" s="368"/>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B72" s="442"/>
-      <c r="D72" s="448"/>
-      <c r="E72" s="448" t="s">
-        <v>185</v>
-      </c>
-      <c r="F72" s="448"/>
-      <c r="G72" s="448"/>
-      <c r="H72" s="448"/>
-      <c r="I72" s="448"/>
-      <c r="J72" s="341"/>
-      <c r="K72" s="341"/>
-      <c r="L72" s="368"/>
-    </row>
-    <row r="73" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="469" t="s">
-        <v>182</v>
-      </c>
-      <c r="C73" s="443"/>
-      <c r="D73" s="443"/>
-      <c r="E73" s="444"/>
-      <c r="F73" s="444"/>
-      <c r="G73" s="444"/>
-      <c r="H73" s="445"/>
-      <c r="I73" s="445"/>
-      <c r="J73" s="446"/>
-      <c r="K73" s="446"/>
-      <c r="L73" s="380"/>
+      <c r="E71" s="354"/>
+      <c r="F71" s="354"/>
+      <c r="G71" s="354"/>
+      <c r="H71" s="355"/>
+      <c r="I71" s="341"/>
+      <c r="J71" s="341"/>
+      <c r="K71" s="341"/>
+      <c r="L71" s="367"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="436"/>
+      <c r="D72" s="442"/>
+      <c r="E72" s="442" t="s">
+        <v>181</v>
+      </c>
+      <c r="F72" s="442"/>
+      <c r="G72" s="442"/>
+      <c r="H72" s="442"/>
+      <c r="I72" s="442"/>
+      <c r="J72" s="340"/>
+      <c r="K72" s="340"/>
+      <c r="L72" s="367"/>
+    </row>
+    <row r="73" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="463" t="s">
+        <v>178</v>
+      </c>
+      <c r="C73" s="437"/>
+      <c r="D73" s="437"/>
+      <c r="E73" s="438"/>
+      <c r="F73" s="438"/>
+      <c r="G73" s="438"/>
+      <c r="H73" s="439"/>
+      <c r="I73" s="439"/>
+      <c r="J73" s="440"/>
+      <c r="K73" s="440"/>
+      <c r="L73" s="379"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -6774,7 +6786,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:Q68"/>
@@ -6783,14 +6795,14 @@
       <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="15" max="15" width="14.5" customWidth="1"/>
-    <col min="16" max="16" width="18.83203125" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" customWidth="1"/>
+    <col min="16" max="16" width="18.875" customWidth="1"/>
+    <col min="17" max="17" width="5.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="218"/>
       <c r="C2" s="219"/>
       <c r="D2" s="219"/>
@@ -6810,7 +6822,7 @@
       </c>
       <c r="Q2" s="222"/>
     </row>
-    <row r="3" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="106"/>
       <c r="C3" s="181"/>
       <c r="D3" s="181"/>
@@ -6845,15 +6857,15 @@
       <c r="K4" s="178"/>
       <c r="L4" s="178"/>
       <c r="M4" s="181"/>
-      <c r="N4" s="520" t="str">
+      <c r="N4" s="511" t="str">
         <f>"CA-"&amp;C9</f>
         <v>CA--</v>
       </c>
-      <c r="O4" s="513"/>
-      <c r="P4" s="513"/>
+      <c r="O4" s="504"/>
+      <c r="P4" s="504"/>
       <c r="Q4" s="97"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="106"/>
       <c r="C5" s="181"/>
       <c r="D5" s="181"/>
@@ -6871,7 +6883,7 @@
       <c r="P5" s="170"/>
       <c r="Q5" s="98"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="106"/>
       <c r="C6" s="181"/>
       <c r="D6" s="181"/>
@@ -6889,7 +6901,7 @@
       <c r="P6" s="175"/>
       <c r="Q6" s="99"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="223" t="s">
         <v>59</v>
       </c>
@@ -6909,7 +6921,7 @@
       <c r="P7" s="179"/>
       <c r="Q7" s="101"/>
     </row>
-    <row r="8" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="106"/>
       <c r="C8" s="181"/>
       <c r="D8" s="181"/>
@@ -6927,7 +6939,7 @@
       <c r="P8" s="178"/>
       <c r="Q8" s="101"/>
     </row>
-    <row r="9" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="223" t="s">
         <v>60</v>
       </c>
@@ -6953,7 +6965,7 @@
       <c r="P9" s="183"/>
       <c r="Q9" s="105"/>
     </row>
-    <row r="10" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="223" t="s">
         <v>63</v>
       </c>
@@ -6980,7 +6992,7 @@
       <c r="P10" s="186"/>
       <c r="Q10" s="105"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="274" t="s">
         <v>65</v>
       </c>
@@ -6994,8 +7006,8 @@
       <c r="H11" s="188"/>
       <c r="I11" s="189"/>
       <c r="J11" s="182"/>
-      <c r="K11" s="521"/>
-      <c r="L11" s="513"/>
+      <c r="K11" s="512"/>
+      <c r="L11" s="504"/>
       <c r="M11" s="190" t="s">
         <v>66</v>
       </c>
@@ -7007,7 +7019,7 @@
       <c r="P11" s="186"/>
       <c r="Q11" s="105"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="223" t="s">
         <v>67</v>
       </c>
@@ -7034,7 +7046,7 @@
       </c>
       <c r="Q12" s="105"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="106"/>
       <c r="C13" s="181"/>
       <c r="D13" s="181"/>
@@ -7049,15 +7061,15 @@
       <c r="M13" s="190" t="s">
         <v>69</v>
       </c>
-      <c r="N13" s="522">
+      <c r="N13" s="513">
         <f>BD!B14</f>
         <v>0</v>
       </c>
-      <c r="O13" s="513"/>
-      <c r="P13" s="513"/>
+      <c r="O13" s="504"/>
+      <c r="P13" s="504"/>
       <c r="Q13" s="105"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="106"/>
       <c r="C14" s="181"/>
       <c r="D14" s="181"/>
@@ -7070,12 +7082,12 @@
       <c r="K14" s="178"/>
       <c r="L14" s="178"/>
       <c r="M14" s="181"/>
-      <c r="N14" s="513"/>
-      <c r="O14" s="513"/>
-      <c r="P14" s="513"/>
+      <c r="N14" s="504"/>
+      <c r="O14" s="504"/>
+      <c r="P14" s="504"/>
       <c r="Q14" s="105"/>
     </row>
-    <row r="15" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="106"/>
       <c r="C15" s="181"/>
       <c r="D15" s="181"/>
@@ -7085,20 +7097,20 @@
       <c r="H15" s="181"/>
       <c r="I15" s="189"/>
       <c r="J15" s="183"/>
-      <c r="K15" s="517" t="s">
+      <c r="K15" s="508" t="s">
         <v>70</v>
       </c>
-      <c r="L15" s="513"/>
-      <c r="M15" s="513"/>
-      <c r="N15" s="518">
+      <c r="L15" s="504"/>
+      <c r="M15" s="504"/>
+      <c r="N15" s="509">
         <f>BD!B15</f>
         <v>0</v>
       </c>
-      <c r="O15" s="519"/>
-      <c r="P15" s="519"/>
+      <c r="O15" s="510"/>
+      <c r="P15" s="510"/>
       <c r="Q15" s="105"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="108" t="s">
         <v>71</v>
       </c>
@@ -7118,49 +7130,49 @@
       <c r="P16" s="178"/>
       <c r="Q16" s="105"/>
     </row>
-    <row r="17" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="109"/>
       <c r="C17" s="180"/>
-      <c r="D17" s="511" t="str">
+      <c r="D17" s="502" t="str">
         <f>"Descripción en Orden de Servicio N°"&amp;C9&amp;" "&amp;C10</f>
         <v>Descripción en Orden de Servicio N°- 0</v>
       </c>
-      <c r="E17" s="511"/>
-      <c r="F17" s="511"/>
-      <c r="G17" s="511"/>
-      <c r="H17" s="511"/>
-      <c r="I17" s="511"/>
-      <c r="J17" s="511"/>
-      <c r="K17" s="511"/>
-      <c r="L17" s="511"/>
-      <c r="M17" s="511"/>
-      <c r="N17" s="511"/>
-      <c r="O17" s="511"/>
-      <c r="P17" s="511"/>
+      <c r="E17" s="502"/>
+      <c r="F17" s="502"/>
+      <c r="G17" s="502"/>
+      <c r="H17" s="502"/>
+      <c r="I17" s="502"/>
+      <c r="J17" s="502"/>
+      <c r="K17" s="502"/>
+      <c r="L17" s="502"/>
+      <c r="M17" s="502"/>
+      <c r="N17" s="502"/>
+      <c r="O17" s="502"/>
+      <c r="P17" s="502"/>
       <c r="Q17" s="105"/>
     </row>
-    <row r="18" spans="2:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="110"/>
       <c r="C18" s="194"/>
-      <c r="D18" s="512" t="str">
+      <c r="D18" s="503" t="str">
         <f>"Esta orden de cambio de contrato, tiene como objetivo ajustar el alcance, valor y plazo del Contrato "&amp;BD!B5&amp;" incorporando el alcance de servicio denominado "&amp;BD!B9&amp;" "&amp;BD!B13</f>
         <v xml:space="preserve">Esta orden de cambio de contrato, tiene como objetivo ajustar el alcance, valor y plazo del Contrato  incorporando el alcance de servicio denominado  </v>
       </c>
-      <c r="E18" s="513"/>
-      <c r="F18" s="513"/>
-      <c r="G18" s="513"/>
-      <c r="H18" s="513"/>
-      <c r="I18" s="513"/>
-      <c r="J18" s="513"/>
-      <c r="K18" s="513"/>
-      <c r="L18" s="513"/>
-      <c r="M18" s="513"/>
-      <c r="N18" s="513"/>
-      <c r="O18" s="513"/>
-      <c r="P18" s="513"/>
+      <c r="E18" s="504"/>
+      <c r="F18" s="504"/>
+      <c r="G18" s="504"/>
+      <c r="H18" s="504"/>
+      <c r="I18" s="504"/>
+      <c r="J18" s="504"/>
+      <c r="K18" s="504"/>
+      <c r="L18" s="504"/>
+      <c r="M18" s="504"/>
+      <c r="N18" s="504"/>
+      <c r="O18" s="504"/>
+      <c r="P18" s="504"/>
       <c r="Q18" s="105"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="109"/>
       <c r="C19" s="194"/>
       <c r="D19" s="195"/>
@@ -7178,7 +7190,7 @@
       <c r="P19" s="195"/>
       <c r="Q19" s="105"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="111" t="s">
         <v>72</v>
       </c>
@@ -7198,7 +7210,7 @@
       <c r="P20" s="177"/>
       <c r="Q20" s="105"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="114"/>
       <c r="C21" s="225"/>
       <c r="D21" s="194"/>
@@ -7216,7 +7228,7 @@
       <c r="P21" s="177"/>
       <c r="Q21" s="105"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="114"/>
       <c r="C22" s="225"/>
       <c r="D22" s="192" t="s">
@@ -7242,7 +7254,7 @@
       <c r="P22" s="183"/>
       <c r="Q22" s="165"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="114"/>
       <c r="C23" s="225"/>
       <c r="D23" s="183"/>
@@ -7260,7 +7272,7 @@
       <c r="P23" s="177"/>
       <c r="Q23" s="165"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="114"/>
       <c r="C24" s="225"/>
       <c r="D24" s="226" t="s">
@@ -7288,7 +7300,7 @@
       <c r="P24" s="230"/>
       <c r="Q24" s="165"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="114"/>
       <c r="C25" s="225"/>
       <c r="D25" s="194"/>
@@ -7306,7 +7318,7 @@
       <c r="P25" s="232"/>
       <c r="Q25" s="165"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="114"/>
       <c r="C26" s="225"/>
       <c r="D26" s="203" t="s">
@@ -7332,7 +7344,7 @@
       <c r="P26" s="234"/>
       <c r="Q26" s="165"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="114"/>
       <c r="C27" s="225"/>
       <c r="D27" s="183"/>
@@ -7350,7 +7362,7 @@
       <c r="P27" s="177"/>
       <c r="Q27" s="165"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="111" t="s">
         <v>84</v>
       </c>
@@ -7370,7 +7382,7 @@
       <c r="P28" s="174"/>
       <c r="Q28" s="112"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="114"/>
       <c r="C29" s="225"/>
       <c r="D29" s="177"/>
@@ -7392,7 +7404,7 @@
       </c>
       <c r="Q29" s="113"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="114"/>
       <c r="D30" s="235" t="s">
         <v>86</v>
@@ -7421,7 +7433,7 @@
       </c>
       <c r="Q30" s="113"/>
     </row>
-    <row r="31" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="114"/>
       <c r="D31" s="156">
         <v>1</v>
@@ -7453,7 +7465,7 @@
       </c>
       <c r="Q31" s="115"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="114"/>
       <c r="C32" s="225"/>
       <c r="D32" s="208"/>
@@ -7474,17 +7486,17 @@
       </c>
       <c r="Q32" s="113"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="114"/>
       <c r="C33" s="225"/>
       <c r="E33" s="271" t="s">
         <v>92</v>
       </c>
-      <c r="F33" s="510">
+      <c r="F33" s="501">
         <f>BD!C19</f>
         <v>0</v>
       </c>
-      <c r="G33" s="510"/>
+      <c r="G33" s="501"/>
       <c r="H33" s="209"/>
       <c r="I33" s="209"/>
       <c r="J33" s="209"/>
@@ -7500,17 +7512,17 @@
       </c>
       <c r="Q33" s="113"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="114"/>
       <c r="C34" s="225"/>
       <c r="E34" s="271" t="s">
         <v>94</v>
       </c>
-      <c r="F34" s="510">
+      <c r="F34" s="501">
         <f>BD!C20</f>
         <v>0</v>
       </c>
-      <c r="G34" s="513"/>
+      <c r="G34" s="504"/>
       <c r="H34" s="211"/>
       <c r="I34" s="211"/>
       <c r="J34" s="211"/>
@@ -7526,17 +7538,17 @@
       </c>
       <c r="Q34" s="113"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="114"/>
       <c r="C35" s="225"/>
       <c r="E35" s="271" t="s">
         <v>96</v>
       </c>
-      <c r="F35" s="510">
+      <c r="F35" s="501">
         <f>BD!C21</f>
         <v>0</v>
       </c>
-      <c r="G35" s="513"/>
+      <c r="G35" s="504"/>
       <c r="H35" s="209"/>
       <c r="I35" s="209"/>
       <c r="J35" s="209"/>
@@ -7552,17 +7564,17 @@
       <c r="P35" s="215"/>
       <c r="Q35" s="113"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="114"/>
       <c r="C36" s="225"/>
       <c r="E36" s="271" t="s">
         <v>98</v>
       </c>
-      <c r="F36" s="510">
+      <c r="F36" s="501">
         <f>F33+F34+F35</f>
         <v>0</v>
       </c>
-      <c r="G36" s="513"/>
+      <c r="G36" s="504"/>
       <c r="H36" s="211"/>
       <c r="I36" s="211"/>
       <c r="J36" s="211"/>
@@ -7574,7 +7586,7 @@
       <c r="P36" s="216"/>
       <c r="Q36" s="105"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="240"/>
       <c r="C37" s="241"/>
       <c r="D37" s="241"/>
@@ -7592,7 +7604,7 @@
       <c r="P37" s="241"/>
       <c r="Q37" s="242"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" s="243"/>
       <c r="C38" s="244"/>
       <c r="D38" s="244"/>
@@ -7610,27 +7622,27 @@
       <c r="P38" s="248"/>
       <c r="Q38" s="249"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B39" s="514" t="s">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B39" s="505" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="515"/>
-      <c r="D39" s="515"/>
-      <c r="E39" s="515"/>
-      <c r="F39" s="515"/>
-      <c r="G39" s="515"/>
-      <c r="H39" s="515"/>
-      <c r="I39" s="515"/>
-      <c r="J39" s="515"/>
-      <c r="K39" s="515"/>
-      <c r="L39" s="515"/>
-      <c r="M39" s="515"/>
-      <c r="N39" s="515"/>
-      <c r="O39" s="515"/>
-      <c r="P39" s="515"/>
-      <c r="Q39" s="516"/>
-    </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C39" s="506"/>
+      <c r="D39" s="506"/>
+      <c r="E39" s="506"/>
+      <c r="F39" s="506"/>
+      <c r="G39" s="506"/>
+      <c r="H39" s="506"/>
+      <c r="I39" s="506"/>
+      <c r="J39" s="506"/>
+      <c r="K39" s="506"/>
+      <c r="L39" s="506"/>
+      <c r="M39" s="506"/>
+      <c r="N39" s="506"/>
+      <c r="O39" s="506"/>
+      <c r="P39" s="506"/>
+      <c r="Q39" s="507"/>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="117"/>
       <c r="C40" s="250"/>
       <c r="D40" s="251"/>
@@ -7648,7 +7660,7 @@
       <c r="P40" s="253"/>
       <c r="Q40" s="118"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" s="119"/>
       <c r="C41" s="180"/>
       <c r="D41" s="254" t="s">
@@ -7670,7 +7682,7 @@
       <c r="P41" s="253"/>
       <c r="Q41" s="120"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" s="119"/>
       <c r="C42" s="250"/>
       <c r="D42" s="251"/>
@@ -7688,7 +7700,7 @@
       <c r="P42" s="253"/>
       <c r="Q42" s="120"/>
     </row>
-    <row r="43" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="119"/>
       <c r="C43" s="180"/>
       <c r="D43" s="254" t="s">
@@ -7710,7 +7722,7 @@
       <c r="P43" s="258"/>
       <c r="Q43" s="118"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" s="119"/>
       <c r="C44" s="180"/>
       <c r="D44" s="250"/>
@@ -7728,7 +7740,7 @@
       <c r="P44" s="253"/>
       <c r="Q44" s="118"/>
     </row>
-    <row r="45" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="119"/>
       <c r="C45" s="180"/>
       <c r="D45" s="166" t="s">
@@ -7750,7 +7762,7 @@
       <c r="P45" s="258"/>
       <c r="Q45" s="120"/>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" s="119"/>
       <c r="C46" s="180"/>
       <c r="D46" s="180"/>
@@ -7768,7 +7780,7 @@
       <c r="P46" s="261"/>
       <c r="Q46" s="120"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" s="164"/>
       <c r="C47" s="180"/>
       <c r="D47" s="262"/>
@@ -7786,7 +7798,7 @@
       <c r="P47" s="263"/>
       <c r="Q47" s="120"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" s="164"/>
       <c r="C48" s="180"/>
       <c r="D48" s="264" t="s">
@@ -7812,7 +7824,7 @@
       <c r="P48" s="261"/>
       <c r="Q48" s="120"/>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B49" s="266"/>
       <c r="C49" s="267"/>
       <c r="D49" s="267"/>
@@ -7830,7 +7842,7 @@
       <c r="P49" s="267"/>
       <c r="Q49" s="269"/>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50" s="243"/>
       <c r="C50" s="244"/>
       <c r="D50" s="244"/>
@@ -7848,7 +7860,7 @@
       <c r="P50" s="248"/>
       <c r="Q50" s="249"/>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B51" s="270" t="s">
         <v>109</v>
       </c>
@@ -7868,7 +7880,7 @@
       <c r="P51" s="103"/>
       <c r="Q51" s="125"/>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B52" s="126"/>
       <c r="C52" s="127"/>
       <c r="D52" s="127"/>
@@ -7886,7 +7898,7 @@
       <c r="P52" s="124"/>
       <c r="Q52" s="125"/>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" s="128" t="s">
         <v>110</v>
       </c>
@@ -7908,7 +7920,7 @@
       <c r="P53" s="100"/>
       <c r="Q53" s="130"/>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B54" s="131" t="s">
         <v>112</v>
       </c>
@@ -7932,7 +7944,7 @@
       <c r="P54" s="100"/>
       <c r="Q54" s="133"/>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B55" s="131" t="s">
         <v>114</v>
       </c>
@@ -7956,7 +7968,7 @@
       <c r="P55" s="100"/>
       <c r="Q55" s="133"/>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B56" s="131"/>
       <c r="C56" s="103"/>
       <c r="D56" s="132"/>
@@ -7974,7 +7986,7 @@
       <c r="P56" s="100"/>
       <c r="Q56" s="133"/>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B57" s="131" t="s">
         <v>116</v>
       </c>
@@ -7996,7 +8008,7 @@
       <c r="P57" s="100"/>
       <c r="Q57" s="133"/>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B58" s="109"/>
       <c r="C58" s="116"/>
       <c r="D58" s="103"/>
@@ -8014,7 +8026,7 @@
       <c r="P58" s="100"/>
       <c r="Q58" s="133"/>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B59" s="108" t="s">
         <v>117</v>
       </c>
@@ -8034,7 +8046,7 @@
       <c r="P59" s="100"/>
       <c r="Q59" s="133"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" s="138"/>
       <c r="C60" s="121"/>
       <c r="D60" s="121"/>
@@ -8052,7 +8064,7 @@
       <c r="P60" s="100"/>
       <c r="Q60" s="99"/>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B61" s="139" t="s">
         <v>118</v>
       </c>
@@ -8076,7 +8088,7 @@
       <c r="P61" s="103"/>
       <c r="Q61" s="143"/>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B62" s="144" t="s">
         <v>112</v>
       </c>
@@ -8091,7 +8103,7 @@
       <c r="I62" s="145" t="s">
         <v>112</v>
       </c>
-      <c r="J62" s="486">
+      <c r="J62" s="480">
         <f>BD!B15</f>
         <v>0</v>
       </c>
@@ -8105,7 +8117,7 @@
       <c r="P62" s="100"/>
       <c r="Q62" s="143"/>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B63" s="144" t="s">
         <v>114</v>
       </c>
@@ -8120,7 +8132,7 @@
       <c r="I63" s="145" t="s">
         <v>114</v>
       </c>
-      <c r="J63" s="486">
+      <c r="J63" s="480">
         <f>BD!B16</f>
         <v>0</v>
       </c>
@@ -8132,7 +8144,7 @@
       <c r="P63" s="100"/>
       <c r="Q63" s="147"/>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B64" s="144"/>
       <c r="C64" s="103"/>
       <c r="D64" s="116"/>
@@ -8150,7 +8162,7 @@
       <c r="P64" s="100"/>
       <c r="Q64" s="143"/>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B65" s="144" t="s">
         <v>116</v>
       </c>
@@ -8174,7 +8186,7 @@
       <c r="P65" s="168"/>
       <c r="Q65" s="143"/>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B66" s="150"/>
       <c r="C66" s="132"/>
       <c r="D66" s="132"/>
@@ -8192,7 +8204,7 @@
       <c r="P66" s="100"/>
       <c r="Q66" s="143"/>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B67" s="109"/>
       <c r="C67" s="102"/>
       <c r="D67" s="102"/>
@@ -8212,7 +8224,7 @@
       <c r="P67" s="151"/>
       <c r="Q67" s="99"/>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B68" s="152"/>
       <c r="C68" s="153"/>
       <c r="D68" s="153"/>

</xml_diff>